<commit_message>
Code adjustments and results adjustments
</commit_message>
<xml_diff>
--- a/data/Output/xlsx/results.xlsx
+++ b/data/Output/xlsx/results.xlsx
@@ -609,13 +609,13 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0.125</v>
+        <v>1</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0.2758190862522522</v>
+        <v>0.2757802710344801</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -624,7 +624,7 @@
         <v>0</v>
       </c>
       <c r="J2">
-        <v>0.2476960667182743</v>
+        <v>0.2476798937108692</v>
       </c>
       <c r="K2" t="s">
         <v>47</v>
@@ -651,13 +651,13 @@
         <v>0</v>
       </c>
       <c r="S2">
-        <v>-2.578691886041252</v>
+        <v>-2.578523513553466</v>
       </c>
       <c r="T2">
         <v>-0</v>
       </c>
       <c r="U2">
-        <v>2.578691886041252</v>
+        <v>2.578523513553466</v>
       </c>
       <c r="V2">
         <v>2.764490036231884</v>
@@ -674,19 +674,19 @@
         <v>105.9164436645103</v>
       </c>
       <c r="C3">
-        <v>47.10654056979374</v>
+        <v>47.10738243223267</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0.125</v>
+        <v>1</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0.3431447329968966</v>
+        <v>0.3431638519279241</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -695,7 +695,7 @@
         <v>0</v>
       </c>
       <c r="J3">
-        <v>0.2881020954038853</v>
+        <v>0.2881100616251468</v>
       </c>
       <c r="K3" t="s">
         <v>47</v>
@@ -722,13 +722,13 @@
         <v>0</v>
       </c>
       <c r="S3">
-        <v>-2.720088453087106</v>
+        <v>-2.720163665405287</v>
       </c>
       <c r="T3">
         <v>-0</v>
       </c>
       <c r="U3">
-        <v>2.720088453087106</v>
+        <v>2.720163665405287</v>
       </c>
       <c r="V3">
         <v>2.740370018115942</v>
@@ -745,19 +745,19 @@
         <v>122.2299783243869</v>
       </c>
       <c r="C4">
-        <v>33.5060983043582</v>
+        <v>33.50656410520624</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>0.125</v>
+        <v>1</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>0.3961672903361316</v>
+        <v>0.3962168548245172</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -766,7 +766,7 @@
         <v>0</v>
       </c>
       <c r="J4">
-        <v>0.3301605545412593</v>
+        <v>0.33018120641142</v>
       </c>
       <c r="K4" t="s">
         <v>47</v>
@@ -793,13 +793,13 @@
         <v>0</v>
       </c>
       <c r="S4">
-        <v>-2.70114221623311</v>
+        <v>-2.701311175357899</v>
       </c>
       <c r="T4">
         <v>-0</v>
       </c>
       <c r="U4">
-        <v>2.70114221623311</v>
+        <v>2.701311175357899</v>
       </c>
       <c r="V4">
         <v>2.701315217391305</v>
@@ -816,28 +816,28 @@
         <v>89.729705482559</v>
       </c>
       <c r="C5">
-        <v>20.00038722319266</v>
+        <v>20.00000822841674</v>
       </c>
       <c r="D5">
-        <v>-7.083792575843172E-06</v>
+        <v>-8.836078093497032E-08</v>
       </c>
       <c r="E5">
-        <v>0.125</v>
+        <v>1</v>
       </c>
       <c r="F5">
-        <v>3.541896287921586E-07</v>
+        <v>4.418039046748516E-09</v>
       </c>
       <c r="G5">
-        <v>-0.2911297485581749</v>
+        <v>-0.291145193183945</v>
       </c>
       <c r="H5">
-        <v>6.356266215299459E-07</v>
+        <v>7.9285868495038E-09</v>
       </c>
       <c r="I5">
         <v>0</v>
       </c>
       <c r="J5">
-        <v>6.313457985108652E-06</v>
+        <v>1.397380953274697E-07</v>
       </c>
       <c r="K5" t="s">
         <v>47</v>
@@ -861,16 +861,16 @@
         <v>0</v>
       </c>
       <c r="R5">
-        <v>7.083792575843172E-06</v>
+        <v>8.836078093497032E-08</v>
       </c>
       <c r="S5">
-        <v>-7.036084595569987E-05</v>
+        <v>-1.557322567548503E-06</v>
       </c>
       <c r="T5">
         <v>-0</v>
       </c>
       <c r="U5">
-        <v>7.036084595569987E-05</v>
+        <v>1.557322567548503E-06</v>
       </c>
       <c r="V5">
         <v>2.70391259057971</v>
@@ -893,7 +893,7 @@
         <v>9.570888597260158</v>
       </c>
       <c r="E6">
-        <v>0.125</v>
+        <v>1</v>
       </c>
       <c r="F6">
         <v>0.4785444298630079</v>
@@ -964,13 +964,13 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>0.125</v>
+        <v>1</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7">
-        <v>0.4163920224027862</v>
+        <v>0.4163950387989465</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -979,7 +979,7 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <v>0.3469947223666593</v>
+        <v>0.3469959791983928</v>
       </c>
       <c r="K7" t="s">
         <v>47</v>
@@ -1006,13 +1006,13 @@
         <v>0</v>
       </c>
       <c r="S7">
-        <v>-3.351485188045559</v>
+        <v>-3.351497329532523</v>
       </c>
       <c r="T7">
         <v>-0.000619780219780219</v>
       </c>
       <c r="U7">
-        <v>3.352104968265339</v>
+        <v>3.352117109752303</v>
       </c>
       <c r="V7">
         <v>3.352118206521739</v>
@@ -1029,28 +1029,28 @@
         <v>121.4558228816549</v>
       </c>
       <c r="C8">
-        <v>51.09701704607299</v>
+        <v>51.09695633863818</v>
       </c>
       <c r="D8">
-        <v>-2.371900527940436</v>
+        <v>-2.371889295868397</v>
       </c>
       <c r="E8">
-        <v>0.125</v>
+        <v>1</v>
       </c>
       <c r="F8">
-        <v>0.1185950263970218</v>
+        <v>0.1185944647934199</v>
       </c>
       <c r="G8">
-        <v>0.8100081293498981</v>
+        <v>0.8100065000603751</v>
       </c>
       <c r="H8">
-        <v>0.2880811304144373</v>
+        <v>0.2880797662138852</v>
       </c>
       <c r="I8">
         <v>0</v>
       </c>
       <c r="J8">
-        <v>0.4910671963242005</v>
+        <v>0.4910670858704626</v>
       </c>
       <c r="K8" t="s">
         <v>47</v>
@@ -1074,16 +1074,16 @@
         <v>0</v>
       </c>
       <c r="R8">
-        <v>2.371900527940436</v>
+        <v>2.371889295868397</v>
       </c>
       <c r="S8">
-        <v>-3.847502881274162</v>
+        <v>-3.847501971859238</v>
       </c>
       <c r="T8">
         <v>-0.1956725274725275</v>
       </c>
       <c r="U8">
-        <v>4.04317540874669</v>
+        <v>4.043174499331766</v>
       </c>
       <c r="V8">
         <v>4.505302536231884</v>
@@ -1106,13 +1106,13 @@
         <v>9.570888597260158</v>
       </c>
       <c r="E9">
-        <v>0.125</v>
+        <v>1</v>
       </c>
       <c r="F9">
         <v>0.4785444298630079</v>
       </c>
       <c r="G9">
-        <v>-1.122520128618319</v>
+        <v>-1.12250361326851</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -1121,7 +1121,7 @@
         <v>0</v>
       </c>
       <c r="J9">
-        <v>0.1173995227551059</v>
+        <v>0.1174132855466139</v>
       </c>
       <c r="K9" t="s">
         <v>47</v>
@@ -1136,10 +1136,10 @@
         <v>0</v>
       </c>
       <c r="O9">
-        <v>0.0001673869142115869</v>
+        <v>2.572754361107599E-06</v>
       </c>
       <c r="P9">
-        <v>9.570721210345946</v>
+        <v>9.570886024505796</v>
       </c>
       <c r="Q9">
         <v>0</v>
@@ -1151,10 +1151,10 @@
         <v>-0</v>
       </c>
       <c r="T9">
-        <v>-1.405899646052821</v>
+        <v>-1.406064460212672</v>
       </c>
       <c r="U9">
-        <v>1.405899646052821</v>
+        <v>1.406064460212672</v>
       </c>
       <c r="V9">
         <v>4.443215126811594</v>
@@ -1177,13 +1177,13 @@
         <v>4.429111402739842</v>
       </c>
       <c r="E10">
-        <v>0.125</v>
+        <v>1</v>
       </c>
       <c r="F10">
         <v>0.2214555701369921</v>
       </c>
       <c r="G10">
-        <v>-0.2994231100942621</v>
+        <v>-0.2994219358709864</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -1192,7 +1192,7 @@
         <v>0</v>
       </c>
       <c r="J10">
-        <v>0.2440881710040949</v>
+        <v>0.2440891495234913</v>
       </c>
       <c r="K10" t="s">
         <v>47</v>
@@ -1207,10 +1207,10 @@
         <v>0</v>
       </c>
       <c r="O10">
-        <v>1.242122556499581E-05</v>
+        <v>7.093727401041861E-07</v>
       </c>
       <c r="P10">
-        <v>4.429098981514278</v>
+        <v>4.429110693367102</v>
       </c>
       <c r="Q10">
         <v>0</v>
@@ -1222,10 +1222,10 @@
         <v>-0</v>
       </c>
       <c r="T10">
-        <v>-2.921479886466743</v>
+        <v>-2.921491598319568</v>
       </c>
       <c r="U10">
-        <v>2.921479886466743</v>
+        <v>2.921491598319568</v>
       </c>
       <c r="V10">
         <v>4.400345108695652</v>
@@ -1248,13 +1248,13 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>0.125</v>
+        <v>1</v>
       </c>
       <c r="F11">
         <v>0</v>
       </c>
       <c r="G11">
-        <v>0.5833105122525338</v>
+        <v>0.5833178818634276</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -1263,7 +1263,7 @@
         <v>0</v>
       </c>
       <c r="J11">
-        <v>0.4860952668437458</v>
+        <v>0.4860983375149515</v>
       </c>
       <c r="K11" t="s">
         <v>47</v>
@@ -1290,13 +1290,13 @@
         <v>0</v>
       </c>
       <c r="S11">
-        <v>-0.4052932313276161</v>
+        <v>-0.4053217716707529</v>
       </c>
       <c r="T11">
         <v>-4.112717582417583</v>
       </c>
       <c r="U11">
-        <v>4.518010813745199</v>
+        <v>4.518039354088335</v>
       </c>
       <c r="V11">
         <v>4.518040307971015</v>
@@ -1313,19 +1313,19 @@
         <v>111.4679819417473</v>
       </c>
       <c r="C12">
-        <v>87.97353384336192</v>
+        <v>87.97339114164625</v>
       </c>
       <c r="D12">
         <v>0</v>
       </c>
       <c r="E12">
-        <v>0.125</v>
+        <v>1</v>
       </c>
       <c r="F12">
         <v>0</v>
       </c>
       <c r="G12">
-        <v>0.7361965562237304</v>
+        <v>0.7362097884893807</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -1334,7 +1334,7 @@
         <v>0</v>
       </c>
       <c r="J12">
-        <v>0.6135027972239124</v>
+        <v>0.6135083106679333</v>
       </c>
       <c r="K12" t="s">
         <v>47</v>
@@ -1361,13 +1361,13 @@
         <v>0</v>
       </c>
       <c r="S12">
-        <v>-0.8290059524356153</v>
+        <v>-0.8290554145674749</v>
       </c>
       <c r="T12">
         <v>-4.674841758241758</v>
       </c>
       <c r="U12">
-        <v>5.503847710677373</v>
+        <v>5.503897172809233</v>
       </c>
       <c r="V12">
         <v>5.503898550724638</v>
@@ -1384,28 +1384,28 @@
         <v>140.0245837966475</v>
       </c>
       <c r="C13">
-        <v>83.82850408118384</v>
+        <v>83.82811406880887</v>
       </c>
       <c r="D13">
-        <v>-4.140636948426824</v>
+        <v>-4.140548588477222</v>
       </c>
       <c r="E13">
-        <v>0.125</v>
+        <v>1</v>
       </c>
       <c r="F13">
-        <v>0.2070318474213412</v>
+        <v>0.2070274294238611</v>
       </c>
       <c r="G13">
-        <v>1.600584442341571</v>
+        <v>1.600573204122853</v>
       </c>
       <c r="H13">
-        <v>0.5797909653564864</v>
+        <v>0.5797785927913192</v>
       </c>
       <c r="I13">
         <v>0</v>
       </c>
       <c r="J13">
-        <v>0.8506618523451341</v>
+        <v>0.8506623249894878</v>
       </c>
       <c r="K13" t="s">
         <v>47</v>
@@ -1429,16 +1429,16 @@
         <v>0</v>
       </c>
       <c r="R13">
-        <v>4.140636948426824</v>
+        <v>4.140548588477222</v>
       </c>
       <c r="S13">
-        <v>-1.072201399232726</v>
+        <v>-1.072204774671102</v>
       </c>
       <c r="T13">
         <v>-5.002887912087912</v>
       </c>
       <c r="U13">
-        <v>6.075089311320638</v>
+        <v>6.075092686759014</v>
       </c>
       <c r="V13">
         <v>6.075093750000001</v>
@@ -1455,19 +1455,19 @@
         <v>133.8330227159034</v>
       </c>
       <c r="C14">
-        <v>57.76431234288609</v>
+        <v>57.76434725306725</v>
       </c>
       <c r="D14">
         <v>0</v>
       </c>
       <c r="E14">
-        <v>0.125</v>
+        <v>1</v>
       </c>
       <c r="F14">
         <v>0</v>
       </c>
       <c r="G14">
-        <v>1.031828532306803</v>
+        <v>1.031830711928773</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -1476,7 +1476,7 @@
         <v>0</v>
       </c>
       <c r="J14">
-        <v>0.8598581092981523</v>
+        <v>0.8598590174739729</v>
       </c>
       <c r="K14" t="s">
         <v>47</v>
@@ -1503,13 +1503,13 @@
         <v>0</v>
       </c>
       <c r="S14">
-        <v>-1.726077351608813</v>
+        <v>-1.726084137496198</v>
       </c>
       <c r="T14">
         <v>-4.69878021978022</v>
       </c>
       <c r="U14">
-        <v>6.424857571389033</v>
+        <v>6.424864357276418</v>
       </c>
       <c r="V14">
         <v>6.424865036231884</v>
@@ -1526,19 +1526,19 @@
         <v>93.56932221264108</v>
       </c>
       <c r="C15">
-        <v>49.13392558484203</v>
+        <v>49.13392656558626</v>
       </c>
       <c r="D15">
         <v>0</v>
       </c>
       <c r="E15">
-        <v>0.125</v>
+        <v>1</v>
       </c>
       <c r="F15">
         <v>0</v>
       </c>
       <c r="G15">
-        <v>0.7306079276652298</v>
+        <v>0.7306121673939387</v>
       </c>
       <c r="H15">
         <v>0</v>
@@ -1547,7 +1547,7 @@
         <v>0</v>
       </c>
       <c r="J15">
-        <v>0.608841932785407</v>
+        <v>0.6088436993390358</v>
       </c>
       <c r="K15" t="s">
         <v>47</v>
@@ -1574,13 +1574,13 @@
         <v>0</v>
       </c>
       <c r="S15">
-        <v>-2.279142064582279</v>
+        <v>-2.279160944206359</v>
       </c>
       <c r="T15">
         <v>-4.227712087912088</v>
       </c>
       <c r="U15">
-        <v>6.506854152494367</v>
+        <v>6.506873032118446</v>
       </c>
       <c r="V15">
         <v>6.50687545289855</v>
@@ -1597,19 +1597,19 @@
         <v>70.86499221514897</v>
       </c>
       <c r="C16">
-        <v>37.73821526193063</v>
+        <v>37.73812184455447</v>
       </c>
       <c r="D16">
-        <v>9.862892345864116</v>
+        <v>9.862893196220611</v>
       </c>
       <c r="E16">
-        <v>0.125</v>
+        <v>1</v>
       </c>
       <c r="F16">
-        <v>0.4931446172932058</v>
+        <v>0.4931446598110306</v>
       </c>
       <c r="G16">
-        <v>-0.7916426392196056</v>
+        <v>-0.7916354698669097</v>
       </c>
       <c r="H16">
         <v>0</v>
@@ -1618,7 +1618,7 @@
         <v>0</v>
       </c>
       <c r="J16">
-        <v>0.2292595717430177</v>
+        <v>0.2292656064641041</v>
       </c>
       <c r="K16" t="s">
         <v>47</v>
@@ -1633,10 +1633,10 @@
         <v>0</v>
       </c>
       <c r="O16">
-        <v>8.968298782585649E-05</v>
+        <v>4.524986705778389E-06</v>
       </c>
       <c r="P16">
-        <v>9.862802662876291</v>
+        <v>9.862888671233906</v>
       </c>
       <c r="Q16">
         <v>0</v>
@@ -1648,10 +1648,10 @@
         <v>-0</v>
       </c>
       <c r="T16">
-        <v>-3.235159767561625</v>
+        <v>-3.235244925562745</v>
       </c>
       <c r="U16">
-        <v>3.235159767561625</v>
+        <v>3.235244925562745</v>
       </c>
       <c r="V16">
         <v>5.916798913043478</v>
@@ -1668,28 +1668,28 @@
         <v>166.4434092688318</v>
       </c>
       <c r="C17">
-        <v>87.0526769912512</v>
+        <v>87.05258782565753</v>
       </c>
       <c r="D17">
-        <v>-4.184912848450345</v>
+        <v>-4.184913538084566</v>
       </c>
       <c r="E17">
-        <v>0.125</v>
+        <v>1</v>
       </c>
       <c r="F17">
-        <v>0.2092456424225173</v>
+        <v>0.2092456769042283</v>
       </c>
       <c r="G17">
-        <v>1.598705701228873</v>
+        <v>1.598709494803799</v>
       </c>
       <c r="H17">
-        <v>0.6965511619890133</v>
+        <v>0.6965512767740842</v>
       </c>
       <c r="I17">
         <v>0</v>
       </c>
       <c r="J17">
-        <v>0.7517970103616244</v>
+        <v>0.7517985431907311</v>
       </c>
       <c r="K17" t="s">
         <v>47</v>
@@ -1713,16 +1713,16 @@
         <v>0</v>
       </c>
       <c r="R17">
-        <v>4.184912848450345</v>
+        <v>4.184913538084566</v>
       </c>
       <c r="S17">
-        <v>-2.920433658773484</v>
+        <v>-2.920442868084405</v>
       </c>
       <c r="T17">
         <v>-1.596398901098901</v>
       </c>
       <c r="U17">
-        <v>4.516832559872385</v>
+        <v>4.516841769183306</v>
       </c>
       <c r="V17">
         <v>4.516841938405797</v>
@@ -1739,28 +1739,28 @@
         <v>128.9514380688834</v>
       </c>
       <c r="C18">
-        <v>51.52594445513207</v>
+        <v>51.52580579481268</v>
       </c>
       <c r="D18">
-        <v>-2.450703476568852</v>
+        <v>-2.450665837139279</v>
       </c>
       <c r="E18">
-        <v>0.125</v>
+        <v>1</v>
       </c>
       <c r="F18">
-        <v>0.1225351738284426</v>
+        <v>0.1225332918569639</v>
       </c>
       <c r="G18">
-        <v>0.9876430365492377</v>
+        <v>0.9876412490563953</v>
       </c>
       <c r="H18">
-        <v>0.3160217375839655</v>
+        <v>0.316016883925394</v>
       </c>
       <c r="I18">
         <v>0</v>
       </c>
       <c r="J18">
-        <v>0.5605368419052027</v>
+        <v>0.5605381194742565</v>
       </c>
       <c r="K18" t="s">
         <v>47</v>
@@ -1784,16 +1784,16 @@
         <v>0</v>
       </c>
       <c r="R18">
-        <v>2.450703476568852</v>
+        <v>2.450665837139279</v>
       </c>
       <c r="S18">
-        <v>-3.854485414457561</v>
+        <v>-3.854495321823256</v>
       </c>
       <c r="T18">
         <v>-0.4923978021978022</v>
       </c>
       <c r="U18">
-        <v>4.346883216655363</v>
+        <v>4.346893124021058</v>
       </c>
       <c r="V18">
         <v>4.353493659420289</v>
@@ -1816,13 +1816,13 @@
         <v>9.570888597260158</v>
       </c>
       <c r="E19">
-        <v>0.125</v>
+        <v>1</v>
       </c>
       <c r="F19">
         <v>0.4785444298630079</v>
       </c>
       <c r="G19">
-        <v>-1.598034012569881</v>
+        <v>-1.598030624329664</v>
       </c>
       <c r="H19">
         <v>0</v>
@@ -1831,7 +1831,7 @@
         <v>0</v>
       </c>
       <c r="J19">
-        <v>0.002986020528251045</v>
+        <v>0.002988844061765045</v>
       </c>
       <c r="K19" t="s">
         <v>47</v>
@@ -1846,10 +1846,10 @@
         <v>0</v>
       </c>
       <c r="O19">
-        <v>3.316607419302786E-05</v>
+        <v>3.721591209718267E-07</v>
       </c>
       <c r="P19">
-        <v>9.570855431185965</v>
+        <v>9.570888225101037</v>
       </c>
       <c r="Q19">
         <v>0</v>
@@ -1861,10 +1861,10 @@
         <v>-0</v>
       </c>
       <c r="T19">
-        <v>-0.03468111964009268</v>
+        <v>-0.03471391355516474</v>
       </c>
       <c r="U19">
-        <v>0.03468111964009268</v>
+        <v>0.03471391355516474</v>
       </c>
       <c r="V19">
         <v>5.965471467391303</v>
@@ -1887,13 +1887,13 @@
         <v>0</v>
       </c>
       <c r="E20">
-        <v>0.125</v>
+        <v>1</v>
       </c>
       <c r="F20">
         <v>0</v>
       </c>
       <c r="G20">
-        <v>0.2179880709614301</v>
+        <v>0.2180012696364086</v>
       </c>
       <c r="H20">
         <v>0</v>
@@ -1902,7 +1902,7 @@
         <v>0</v>
       </c>
       <c r="J20">
-        <v>0.3986790818889053</v>
+        <v>0.3986845813368131</v>
       </c>
       <c r="K20" t="s">
         <v>47</v>
@@ -1929,13 +1929,13 @@
         <v>0</v>
       </c>
       <c r="S20">
-        <v>-4.005702703123265</v>
+        <v>-4.00575795847613</v>
       </c>
       <c r="T20">
         <v>-0</v>
       </c>
       <c r="U20">
-        <v>4.005702703123265</v>
+        <v>4.00575795847613</v>
       </c>
       <c r="V20">
         <v>6.186221014492753</v>
@@ -1952,28 +1952,28 @@
         <v>93.60128767093309</v>
       </c>
       <c r="C21">
-        <v>47.82592947068446</v>
+        <v>47.82565319392014</v>
       </c>
       <c r="D21">
-        <v>-1.74760485000878</v>
+        <v>-1.747547900335359</v>
       </c>
       <c r="E21">
-        <v>0.125</v>
+        <v>1</v>
       </c>
       <c r="F21">
-        <v>0.08738024250043899</v>
+        <v>0.08737739501676793</v>
       </c>
       <c r="G21">
-        <v>0.3916330687059447</v>
+        <v>0.3916281187605861</v>
       </c>
       <c r="H21">
-        <v>0.1635780643007897</v>
+        <v>0.163572733738025</v>
       </c>
       <c r="I21">
         <v>0</v>
       </c>
       <c r="J21">
-        <v>0.3573305015185366</v>
+        <v>0.3573306601091225</v>
       </c>
       <c r="K21" t="s">
         <v>47</v>
@@ -1997,16 +1997,16 @@
         <v>0</v>
       </c>
       <c r="R21">
-        <v>1.74760485000878</v>
+        <v>1.747547900335359</v>
       </c>
       <c r="S21">
-        <v>-3.817581044128112</v>
+        <v>-3.81758273844867</v>
       </c>
       <c r="T21">
         <v>-0</v>
       </c>
       <c r="U21">
-        <v>3.817581044128112</v>
+        <v>3.81758273844867</v>
       </c>
       <c r="V21">
         <v>5.604785778985508</v>
@@ -2026,16 +2026,16 @@
         <v>20</v>
       </c>
       <c r="D22">
-        <v>7.522795095878275</v>
+        <v>7.522354737325383</v>
       </c>
       <c r="E22">
-        <v>0.125</v>
+        <v>1</v>
       </c>
       <c r="F22">
-        <v>0.3761397547939137</v>
+        <v>0.3761177368662691</v>
       </c>
       <c r="G22">
-        <v>-1.546395897301438</v>
+        <v>-1.546343000520817</v>
       </c>
       <c r="H22">
         <v>0</v>
@@ -2062,7 +2062,7 @@
         <v>0</v>
       </c>
       <c r="P22">
-        <v>7.522795095878275</v>
+        <v>7.522354737325383</v>
       </c>
       <c r="Q22">
         <v>0</v>
@@ -2094,19 +2094,19 @@
         <v>126.6537162367117</v>
       </c>
       <c r="C23">
-        <v>57.61397547939138</v>
+        <v>57.61177368662691</v>
       </c>
       <c r="D23">
         <v>0</v>
       </c>
       <c r="E23">
-        <v>0.125</v>
+        <v>1</v>
       </c>
       <c r="F23">
         <v>0</v>
       </c>
       <c r="G23">
-        <v>0.4647191429748561</v>
+        <v>0.4647082704530749</v>
       </c>
       <c r="H23">
         <v>0</v>
@@ -2115,7 +2115,7 @@
         <v>0</v>
       </c>
       <c r="J23">
-        <v>0.4960126721391549</v>
+        <v>0.4960081419217461</v>
       </c>
       <c r="K23" t="s">
         <v>47</v>
@@ -2142,13 +2142,13 @@
         <v>0</v>
       </c>
       <c r="S23">
-        <v>-3.916289919295564</v>
+        <v>-3.916254150764301</v>
       </c>
       <c r="T23">
         <v>-0</v>
       </c>
       <c r="U23">
-        <v>3.916289919295564</v>
+        <v>3.916254150764301</v>
       </c>
       <c r="V23">
         <v>4.774904438405797</v>
@@ -2165,28 +2165,28 @@
         <v>85.12846470743519</v>
       </c>
       <c r="C24">
-        <v>38.03252588291356</v>
+        <v>38.03050293280541</v>
       </c>
       <c r="D24">
-        <v>-0.0004408238318043267</v>
+        <v>-1.234185405829535E-05</v>
       </c>
       <c r="E24">
-        <v>0.125</v>
+        <v>1</v>
       </c>
       <c r="F24">
-        <v>2.204119159021634E-05</v>
+        <v>6.170927029147677E-07</v>
       </c>
       <c r="G24">
-        <v>0.3684094989080338</v>
+        <v>0.368377904220417</v>
       </c>
       <c r="H24">
-        <v>3.752665600795097E-05</v>
+        <v>1.050643087625912E-06</v>
       </c>
       <c r="I24">
         <v>0</v>
       </c>
       <c r="J24">
-        <v>0.3069787219858957</v>
+        <v>0.3069807558714387</v>
       </c>
       <c r="K24" t="s">
         <v>47</v>
@@ -2210,16 +2210,16 @@
         <v>0</v>
       </c>
       <c r="R24">
-        <v>0.0004408238318043267</v>
+        <v>1.234185405829535E-05</v>
       </c>
       <c r="S24">
-        <v>-3.606064352750907</v>
+        <v>-3.606088244707024</v>
       </c>
       <c r="T24">
         <v>-0</v>
       </c>
       <c r="U24">
-        <v>3.606064352750907</v>
+        <v>3.606088244707024</v>
       </c>
       <c r="V24">
         <v>3.606088768115942</v>
@@ -2242,7 +2242,7 @@
         <v>0</v>
       </c>
       <c r="E25">
-        <v>0.125</v>
+        <v>1</v>
       </c>
       <c r="F25">
         <v>0</v>

</xml_diff>

<commit_message>
Reverting all what was done in test #1
</commit_message>
<xml_diff>
--- a/data/Output/xlsx/results.xlsx
+++ b/data/Output/xlsx/results.xlsx
@@ -615,7 +615,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0.06935292332563825</v>
+        <v>-0.3102236102782091</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -624,7 +624,7 @@
         <v>0</v>
       </c>
       <c r="J2">
-        <v>0.1616684988321851</v>
+        <v>0.003511609830582043</v>
       </c>
       <c r="K2" t="s">
         <v>47</v>
@@ -651,13 +651,13 @@
         <v>0</v>
       </c>
       <c r="S2">
-        <v>-1.683083836132099</v>
+        <v>-0.03655835111570035</v>
       </c>
       <c r="T2">
         <v>-0</v>
       </c>
       <c r="U2">
-        <v>1.683083836132099</v>
+        <v>0.03655835111570035</v>
       </c>
       <c r="V2">
         <v>2.764490036231884</v>
@@ -674,7 +674,7 @@
         <v>105.9164436645103</v>
       </c>
       <c r="C3">
-        <v>58.23625314521874</v>
+        <v>59.81720824442149</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -686,7 +686,7 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0.3221948435380977</v>
+        <v>0.06528219984543301</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -695,7 +695,7 @@
         <v>0</v>
       </c>
       <c r="J3">
-        <v>0.2793729747960524</v>
+        <v>0.1723260399241088</v>
       </c>
       <c r="K3" t="s">
         <v>47</v>
@@ -722,13 +722,13 @@
         <v>0</v>
       </c>
       <c r="S3">
-        <v>-2.637673293496946</v>
+        <v>-1.626999868594065</v>
       </c>
       <c r="T3">
         <v>-0</v>
       </c>
       <c r="U3">
-        <v>2.637673293496946</v>
+        <v>1.626999868594065</v>
       </c>
       <c r="V3">
         <v>2.740370018115942</v>
@@ -745,7 +745,7 @@
         <v>122.2299783243869</v>
       </c>
       <c r="C4">
-        <v>55.47216743809381</v>
+        <v>51.68220890145116</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -757,7 +757,7 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <v>0.327053697937906</v>
+        <v>0.3483097607009766</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -766,7 +766,7 @@
         <v>0</v>
       </c>
       <c r="J4">
-        <v>0.301363224375332</v>
+        <v>0.3102199171932781</v>
       </c>
       <c r="K4" t="s">
         <v>47</v>
@@ -793,13 +793,13 @@
         <v>0</v>
       </c>
       <c r="S4">
-        <v>-2.465542647610902</v>
+        <v>-2.538001899746587</v>
       </c>
       <c r="T4">
         <v>-0</v>
       </c>
       <c r="U4">
-        <v>2.465542647610902</v>
+        <v>2.538001899746587</v>
       </c>
       <c r="V4">
         <v>2.701315217391305</v>
@@ -816,7 +816,7 @@
         <v>89.729705482559</v>
       </c>
       <c r="C5">
-        <v>52.88846186342304</v>
+        <v>38.99219940271823</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -828,7 +828,7 @@
         <v>0</v>
       </c>
       <c r="G5">
-        <v>0.247552619231831</v>
+        <v>-0.280623952189323</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -837,7 +837,7 @@
         <v>0</v>
       </c>
       <c r="J5">
-        <v>0.2244575648815798</v>
+        <v>0.004383993456098986</v>
       </c>
       <c r="K5" t="s">
         <v>47</v>
@@ -864,13 +864,13 @@
         <v>0</v>
       </c>
       <c r="S5">
-        <v>-2.50148558578751</v>
+        <v>-0.04885777159885044</v>
       </c>
       <c r="T5">
         <v>-0</v>
       </c>
       <c r="U5">
-        <v>2.50148558578751</v>
+        <v>0.04885777159885044</v>
       </c>
       <c r="V5">
         <v>2.70391259057971</v>
@@ -887,7 +887,7 @@
         <v>77.99005802293598</v>
       </c>
       <c r="C6">
-        <v>50.26709075908605</v>
+        <v>38.74791054472398</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -899,7 +899,7 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>-0.03249719635035951</v>
+        <v>-0.2443879286041725</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -908,7 +908,7 @@
         <v>0</v>
       </c>
       <c r="J6">
-        <v>0.09138491665269578</v>
+        <v>0.003097111546940342</v>
       </c>
       <c r="K6" t="s">
         <v>47</v>
@@ -935,13 +935,13 @@
         <v>0</v>
       </c>
       <c r="S6">
-        <v>-1.171750848368654</v>
+        <v>-0.039711619986608</v>
       </c>
       <c r="T6">
         <v>-0</v>
       </c>
       <c r="U6">
-        <v>1.171750848368654</v>
+        <v>0.039711619986608</v>
       </c>
       <c r="V6">
         <v>2.690738224637681</v>
@@ -958,7 +958,7 @@
         <v>103.5154703243746</v>
       </c>
       <c r="C7">
-        <v>49.03918289791443</v>
+        <v>38.54935244479094</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -970,7 +970,7 @@
         <v>0</v>
       </c>
       <c r="G7">
-        <v>0.2860480839138936</v>
+        <v>-0.05167717441882491</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -979,7 +979,7 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <v>0.2926847479962875</v>
+        <v>0.1519658903576547</v>
       </c>
       <c r="K7" t="s">
         <v>47</v>
@@ -1006,13 +1006,13 @@
         <v>0</v>
       </c>
       <c r="S7">
-        <v>-2.826829557344303</v>
+        <v>-1.467430259851106</v>
       </c>
       <c r="T7">
         <v>-0.000619780219780219</v>
       </c>
       <c r="U7">
-        <v>2.827449337564083</v>
+        <v>1.468050040070886</v>
       </c>
       <c r="V7">
         <v>3.352118206521739</v>
@@ -1029,7 +1029,7 @@
         <v>121.4558228816549</v>
       </c>
       <c r="C8">
-        <v>46.07687547523333</v>
+        <v>31.21220114553541</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1041,7 +1041,7 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <v>0.5235982219619248</v>
+        <v>0.4280462598895027</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -1050,7 +1050,7 @@
         <v>0</v>
       </c>
       <c r="J8">
-        <v>0.4917635392518938</v>
+        <v>0.4519502217217179</v>
       </c>
       <c r="K8" t="s">
         <v>47</v>
@@ -1077,13 +1077,13 @@
         <v>0</v>
       </c>
       <c r="S8">
-        <v>-3.853236183401404</v>
+        <v>-3.525435370022786</v>
       </c>
       <c r="T8">
         <v>-0.1956725274725275</v>
       </c>
       <c r="U8">
-        <v>4.048908710873931</v>
+        <v>3.721107897495313</v>
       </c>
       <c r="V8">
         <v>4.505302536231884</v>
@@ -1100,19 +1100,19 @@
         <v>83.50490953228045</v>
       </c>
       <c r="C9">
-        <v>42.03897014140174</v>
+        <v>13.58502429542148</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>6.504631141470997</v>
       </c>
       <c r="E9">
         <v>1</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>0.3252315570735498</v>
       </c>
       <c r="G9">
-        <v>0.4399305451164979</v>
+        <v>-0.8765221351827451</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -1121,7 +1121,7 @@
         <v>0</v>
       </c>
       <c r="J9">
-        <v>0.3688195323969718</v>
+        <v>0.06635029916973001</v>
       </c>
       <c r="K9" t="s">
         <v>47</v>
@@ -1136,10 +1136,10 @@
         <v>0</v>
       </c>
       <c r="O9">
-        <v>0</v>
+        <v>0.6114993896827655</v>
       </c>
       <c r="P9">
-        <v>0</v>
+        <v>5.893131751788231</v>
       </c>
       <c r="Q9">
         <v>0</v>
@@ -1148,13 +1148,13 @@
         <v>0</v>
       </c>
       <c r="S9">
-        <v>-3.010673664828675</v>
+        <v>-0</v>
       </c>
       <c r="T9">
-        <v>-1.406067032967033</v>
+        <v>-0.7945676432842671</v>
       </c>
       <c r="U9">
-        <v>4.416740697795708</v>
+        <v>0.7945676432842671</v>
       </c>
       <c r="V9">
         <v>4.443215126811594</v>
@@ -1171,19 +1171,19 @@
         <v>83.54949562883922</v>
       </c>
       <c r="C10">
-        <v>38.88400774849005</v>
+        <v>46.10818000277646</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>6.460424613588851</v>
       </c>
       <c r="E10">
         <v>1</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>0.3230212306794426</v>
       </c>
       <c r="G10">
-        <v>0.1533101637033675</v>
+        <v>-0.5089531785430129</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -1192,7 +1192,7 @@
         <v>0</v>
       </c>
       <c r="J10">
-        <v>0.2477025420885789</v>
+        <v>0.2391949748607684</v>
       </c>
       <c r="K10" t="s">
         <v>47</v>
@@ -1207,10 +1207,10 @@
         <v>0</v>
       </c>
       <c r="O10">
-        <v>0</v>
+        <v>0.05857885668394358</v>
       </c>
       <c r="P10">
-        <v>0</v>
+        <v>6.401845756904907</v>
       </c>
       <c r="Q10">
         <v>0</v>
@@ -1219,13 +1219,13 @@
         <v>0</v>
       </c>
       <c r="S10">
-        <v>-0.04324781699945657</v>
+        <v>-0</v>
       </c>
       <c r="T10">
-        <v>-2.921492307692308</v>
+        <v>-2.862913451008365</v>
       </c>
       <c r="U10">
-        <v>2.964740124691765</v>
+        <v>2.862913451008365</v>
       </c>
       <c r="V10">
         <v>4.400345108695652</v>
@@ -1242,7 +1242,7 @@
         <v>107.5905496651075</v>
       </c>
       <c r="C11">
-        <v>38.83868724836319</v>
+        <v>78.41030307072072</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -1254,7 +1254,7 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <v>0.5804470063286838</v>
+        <v>0.5064483076277337</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -1263,7 +1263,7 @@
         <v>0</v>
       </c>
       <c r="J11">
-        <v>0.484902139375475</v>
+        <v>0.4540693482500791</v>
       </c>
       <c r="K11" t="s">
         <v>47</v>
@@ -1290,13 +1290,13 @@
         <v>0</v>
       </c>
       <c r="S11">
-        <v>-0.3942037121088315</v>
+        <v>-0.1076284392677893</v>
       </c>
       <c r="T11">
         <v>-4.112717582417583</v>
       </c>
       <c r="U11">
-        <v>4.506921294526414</v>
+        <v>4.220346021685372</v>
       </c>
       <c r="V11">
         <v>4.518040307971015</v>
@@ -1313,7 +1313,7 @@
         <v>111.4679819417473</v>
       </c>
       <c r="C12">
-        <v>38.42559103625004</v>
+        <v>77.87216087438178</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -1325,7 +1325,7 @@
         <v>0</v>
       </c>
       <c r="G12">
-        <v>0.6846594013024477</v>
+        <v>0.6534817408827137</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -1334,7 +1334,7 @@
         <v>0</v>
       </c>
       <c r="J12">
-        <v>0.592028982673378</v>
+        <v>0.5790382908318221</v>
       </c>
       <c r="K12" t="s">
         <v>47</v>
@@ -1361,13 +1361,13 @@
         <v>0</v>
       </c>
       <c r="S12">
-        <v>-0.6363603677891057</v>
+        <v>-0.5198184548984184</v>
       </c>
       <c r="T12">
         <v>-4.674841758241758</v>
       </c>
       <c r="U12">
-        <v>5.311202126030864</v>
+        <v>5.194660213140176</v>
       </c>
       <c r="V12">
         <v>5.503898550724638</v>
@@ -1384,7 +1384,7 @@
         <v>140.0245837966475</v>
       </c>
       <c r="C13">
-        <v>37.75873263436863</v>
+        <v>75.2730685998897</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -1396,7 +1396,7 @@
         <v>0</v>
       </c>
       <c r="G13">
-        <v>0.8894208291384192</v>
+        <v>1.011564887143696</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -1405,7 +1405,7 @@
         <v>0</v>
       </c>
       <c r="J13">
-        <v>0.7959232490756902</v>
+        <v>0.846816606577889</v>
       </c>
       <c r="K13" t="s">
         <v>47</v>
@@ -1432,13 +1432,13 @@
         <v>0</v>
       </c>
       <c r="S13">
-        <v>-0.6812800211057342</v>
+        <v>-1.044740180188295</v>
       </c>
       <c r="T13">
         <v>-5.002887912087912</v>
       </c>
       <c r="U13">
-        <v>5.684167933193646</v>
+        <v>6.047628092276207</v>
       </c>
       <c r="V13">
         <v>6.075093750000001</v>
@@ -1455,28 +1455,28 @@
         <v>133.8330227159034</v>
       </c>
       <c r="C14">
-        <v>37.04480177207009</v>
+        <v>70.04936769894822</v>
       </c>
       <c r="D14">
-        <v>-16</v>
+        <v>0</v>
       </c>
       <c r="E14">
         <v>1</v>
       </c>
       <c r="F14">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="G14">
-        <v>2.960122565132423</v>
+        <v>1.015491394397412</v>
       </c>
       <c r="H14">
-        <v>2.141328363454454</v>
+        <v>0</v>
       </c>
       <c r="I14">
         <v>0</v>
       </c>
       <c r="J14">
-        <v>0.771093804869471</v>
+        <v>0.8530509685025724</v>
       </c>
       <c r="K14" t="s">
         <v>47</v>
@@ -1500,16 +1500,16 @@
         <v>0</v>
       </c>
       <c r="R14">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="S14">
-        <v>-1.062830698224114</v>
+        <v>-1.675214413169249</v>
       </c>
       <c r="T14">
         <v>-4.69878021978022</v>
       </c>
       <c r="U14">
-        <v>5.761610918004334</v>
+        <v>6.373994632949469</v>
       </c>
       <c r="V14">
         <v>6.424865036231884</v>
@@ -1526,7 +1526,7 @@
         <v>93.56932221264108</v>
       </c>
       <c r="C15">
-        <v>19.16422248564662</v>
+        <v>61.67329563310198</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -1538,7 +1538,7 @@
         <v>0</v>
       </c>
       <c r="G15">
-        <v>0.7258814405555257</v>
+        <v>0.6253477224934187</v>
       </c>
       <c r="H15">
         <v>0</v>
@@ -1547,7 +1547,7 @@
         <v>0</v>
       </c>
       <c r="J15">
-        <v>0.6068725631563636</v>
+        <v>0.5649835139638191</v>
       </c>
       <c r="K15" t="s">
         <v>47</v>
@@ -1574,13 +1574,13 @@
         <v>0</v>
       </c>
       <c r="S15">
-        <v>-2.258094892469951</v>
+        <v>-1.810415586881421</v>
       </c>
       <c r="T15">
         <v>-4.227712087912088</v>
       </c>
       <c r="U15">
-        <v>6.485806980382039</v>
+        <v>6.038127674793508</v>
       </c>
       <c r="V15">
         <v>6.50687545289855</v>
@@ -1597,19 +1597,19 @@
         <v>70.86499221514897</v>
       </c>
       <c r="C16">
-        <v>16.79790675086768</v>
+        <v>52.62121769869488</v>
       </c>
       <c r="D16">
-        <v>43.181351489862</v>
+        <v>7.475756460261024</v>
       </c>
       <c r="E16">
         <v>1</v>
       </c>
       <c r="F16">
-        <v>2.1590675744931</v>
+        <v>0.3737878230130512</v>
       </c>
       <c r="G16">
-        <v>-3.733728859082521</v>
+        <v>-0.5901451629441445</v>
       </c>
       <c r="H16">
         <v>0</v>
@@ -1618,7 +1618,7 @@
         <v>0</v>
       </c>
       <c r="J16">
-        <v>0.1386334030507572</v>
+        <v>0.2280097693561362</v>
       </c>
       <c r="K16" t="s">
         <v>47</v>
@@ -1633,10 +1633,10 @@
         <v>0</v>
       </c>
       <c r="O16">
-        <v>1.278946363266797</v>
+        <v>0.01772606941523147</v>
       </c>
       <c r="P16">
-        <v>41.90240512659521</v>
+        <v>7.458030390845793</v>
       </c>
       <c r="Q16">
         <v>0</v>
@@ -1648,10 +1648,10 @@
         <v>-0</v>
       </c>
       <c r="T16">
-        <v>-1.956303087282653</v>
+        <v>-3.217523381134219</v>
       </c>
       <c r="U16">
-        <v>1.956303087282653</v>
+        <v>3.217523381134219</v>
       </c>
       <c r="V16">
         <v>5.916798913043478</v>
@@ -1668,7 +1668,7 @@
         <v>166.4434092688318</v>
       </c>
       <c r="C17">
-        <v>62.04875596018194</v>
+        <v>90</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -1680,7 +1680,7 @@
         <v>0</v>
       </c>
       <c r="G17">
-        <v>0.8718559326866198</v>
+        <v>0.8796003027776238</v>
       </c>
       <c r="H17">
         <v>0</v>
@@ -1689,7 +1689,7 @@
         <v>0</v>
       </c>
       <c r="J17">
-        <v>0.7391725909644414</v>
+        <v>0.7423994118356929</v>
       </c>
       <c r="K17" t="s">
         <v>47</v>
@@ -1716,13 +1716,13 @@
         <v>0</v>
       </c>
       <c r="S17">
-        <v>-2.844585540469246</v>
+        <v>-2.863972435302911</v>
       </c>
       <c r="T17">
         <v>-1.596398901098901</v>
       </c>
       <c r="U17">
-        <v>4.440984441568147</v>
+        <v>4.460371336401812</v>
       </c>
       <c r="V17">
         <v>4.516841938405797</v>
@@ -1739,28 +1739,28 @@
         <v>128.9514380688834</v>
       </c>
       <c r="C18">
-        <v>59.06784158595282</v>
+        <v>75.68013782348544</v>
       </c>
       <c r="D18">
-        <v>-16</v>
+        <v>0</v>
       </c>
       <c r="E18">
         <v>1</v>
       </c>
       <c r="F18">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="G18">
-        <v>2.727399243105152</v>
+        <v>0.6398642749122446</v>
       </c>
       <c r="H18">
-        <v>2.063223009102134</v>
+        <v>0</v>
       </c>
       <c r="I18">
         <v>0</v>
       </c>
       <c r="J18">
-        <v>0.5574347315042634</v>
+        <v>0.5473047485497745</v>
       </c>
       <c r="K18" t="s">
         <v>47</v>
@@ -1784,16 +1784,16 @@
         <v>0</v>
       </c>
       <c r="R18">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="S18">
-        <v>-3.830428990989975</v>
+        <v>-3.751872418793567</v>
       </c>
       <c r="T18">
         <v>-0.4923978021978022</v>
       </c>
       <c r="U18">
-        <v>4.322826793187777</v>
+        <v>4.244270220991369</v>
       </c>
       <c r="V18">
         <v>4.353493659420289</v>
@@ -1810,7 +1810,7 @@
         <v>86.09931164964732</v>
       </c>
       <c r="C19">
-        <v>38.28702484292019</v>
+        <v>56.9207757295176</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -1822,7 +1822,7 @@
         <v>0</v>
       </c>
       <c r="G19">
-        <v>0.2888448884020659</v>
+        <v>-0.4849647841108055</v>
       </c>
       <c r="H19">
         <v>0</v>
@@ -1831,7 +1831,7 @@
         <v>0</v>
       </c>
       <c r="J19">
-        <v>0.3771635303381956</v>
+        <v>0.05474283345783239</v>
       </c>
       <c r="K19" t="s">
         <v>47</v>
@@ -1858,13 +1858,13 @@
         <v>0</v>
       </c>
       <c r="S19">
-        <v>-4.345849543563906</v>
+        <v>-0.6010960640895577</v>
       </c>
       <c r="T19">
         <v>-0.03471428571428571</v>
       </c>
       <c r="U19">
-        <v>4.380563829278192</v>
+        <v>0.6358103498038434</v>
       </c>
       <c r="V19">
         <v>5.965471467391303</v>
@@ -1881,7 +1881,7 @@
         <v>99.52787598991144</v>
       </c>
       <c r="C20">
-        <v>33.73289729486633</v>
+        <v>53.91529540906982</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -1893,7 +1893,7 @@
         <v>0</v>
       </c>
       <c r="G20">
-        <v>0.6340872277148202</v>
+        <v>-0.3314358803587044</v>
       </c>
       <c r="H20">
         <v>0</v>
@@ -1902,7 +1902,7 @@
         <v>0</v>
       </c>
       <c r="J20">
-        <v>0.5720537305361512</v>
+        <v>0.169752435505516</v>
       </c>
       <c r="K20" t="s">
         <v>47</v>
@@ -1929,13 +1929,13 @@
         <v>0</v>
       </c>
       <c r="S20">
-        <v>-5.747673451748704</v>
+        <v>-1.705576792603539</v>
       </c>
       <c r="T20">
         <v>-0</v>
       </c>
       <c r="U20">
-        <v>5.747673451748704</v>
+        <v>1.705576792603539</v>
       </c>
       <c r="V20">
         <v>6.186221014492753</v>
@@ -1952,7 +1952,7 @@
         <v>93.60128767093309</v>
       </c>
       <c r="C21">
-        <v>27.70976240686909</v>
+        <v>45.38741144605212</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -1964,7 +1964,7 @@
         <v>0</v>
       </c>
       <c r="G21">
-        <v>0.2475964061971627</v>
+        <v>-0.2909234520802559</v>
       </c>
       <c r="H21">
         <v>0</v>
@@ -1973,7 +1973,7 @@
         <v>0</v>
       </c>
       <c r="J21">
-        <v>0.3654727522652065</v>
+        <v>0.1410894779829487</v>
       </c>
       <c r="K21" t="s">
         <v>47</v>
@@ -2000,13 +2000,13 @@
         <v>0</v>
       </c>
       <c r="S21">
-        <v>-3.904569705815065</v>
+        <v>-1.507345480961397</v>
       </c>
       <c r="T21">
         <v>-0</v>
       </c>
       <c r="U21">
-        <v>3.904569705815065</v>
+        <v>1.507345480961397</v>
       </c>
       <c r="V21">
         <v>5.604785778985508</v>
@@ -2023,7 +2023,7 @@
         <v>100.1017244434446</v>
       </c>
       <c r="C22">
-        <v>23.61806335417557</v>
+        <v>37.85068404124514</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -2035,7 +2035,7 @@
         <v>0</v>
       </c>
       <c r="G22">
-        <v>0.4552103296282416</v>
+        <v>-0.1879398448635849</v>
       </c>
       <c r="H22">
         <v>0</v>
@@ -2044,7 +2044,7 @@
         <v>0</v>
       </c>
       <c r="J22">
-        <v>0.4574802136879814</v>
+        <v>0.189500974316387</v>
       </c>
       <c r="K22" t="s">
         <v>47</v>
@@ -2071,13 +2071,13 @@
         <v>0</v>
       </c>
       <c r="S22">
-        <v>-4.570153173998996</v>
+        <v>-1.893084013986703</v>
       </c>
       <c r="T22">
         <v>-0</v>
       </c>
       <c r="U22">
-        <v>4.570153173998996</v>
+        <v>1.893084013986703</v>
       </c>
       <c r="V22">
         <v>5.350741847826087</v>
@@ -2094,7 +2094,7 @@
         <v>126.6537162367117</v>
       </c>
       <c r="C23">
-        <v>18.828882260836</v>
+        <v>28.38526397131162</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -2106,7 +2106,7 @@
         <v>0</v>
       </c>
       <c r="G23">
-        <v>0.171065435261843</v>
+        <v>0.3524813871803485</v>
       </c>
       <c r="H23">
         <v>0</v>
@@ -2115,7 +2115,7 @@
         <v>0</v>
       </c>
       <c r="J23">
-        <v>0.3736569605920662</v>
+        <v>0.4492469405581101</v>
       </c>
       <c r="K23" t="s">
         <v>47</v>
@@ -2142,13 +2142,13 @@
         <v>0</v>
       </c>
       <c r="S23">
-        <v>-2.950225004797438</v>
+        <v>-3.547049023958224</v>
       </c>
       <c r="T23">
         <v>-0</v>
       </c>
       <c r="U23">
-        <v>2.950225004797438</v>
+        <v>3.547049023958224</v>
       </c>
       <c r="V23">
         <v>4.774904438405797</v>
@@ -2165,28 +2165,28 @@
         <v>85.12846470743519</v>
       </c>
       <c r="C24">
-        <v>15.73726557401276</v>
+        <v>10.65001885152051</v>
       </c>
       <c r="D24">
-        <v>-2.02572209643081</v>
+        <v>0</v>
       </c>
       <c r="E24">
         <v>1</v>
       </c>
       <c r="F24">
-        <v>0.1012861048215405</v>
+        <v>0</v>
       </c>
       <c r="G24">
-        <v>0.5087608947360255</v>
+        <v>-0.3513378968690586</v>
       </c>
       <c r="H24">
-        <v>0.1724466119930819</v>
+        <v>0</v>
       </c>
       <c r="I24">
         <v>0</v>
       </c>
       <c r="J24">
-        <v>0.2936213513571113</v>
+        <v>0.007099609852110451</v>
       </c>
       <c r="K24" t="s">
         <v>47</v>
@@ -2210,16 +2210,16 @@
         <v>0</v>
       </c>
       <c r="R24">
-        <v>2.02572209643081</v>
+        <v>0</v>
       </c>
       <c r="S24">
-        <v>-3.449155959363452</v>
+        <v>-0.08339877708954342</v>
       </c>
       <c r="T24">
         <v>-0</v>
       </c>
       <c r="U24">
-        <v>3.449155959363452</v>
+        <v>0.08339877708954342</v>
       </c>
       <c r="V24">
         <v>3.606088768115942</v>
@@ -2236,7 +2236,7 @@
         <v>99.71725698729442</v>
       </c>
       <c r="C25">
-        <v>10</v>
+        <v>10.23302496607279</v>
       </c>
       <c r="D25">
         <v>0</v>

</xml_diff>

<commit_message>
Final code adjustments + hyperparameters and plot + repo cleaning
</commit_message>
<xml_diff>
--- a/data/Output/xlsx/results.xlsx
+++ b/data/Output/xlsx/results.xlsx
@@ -621,7 +621,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0.1040096728322466</v>
+        <v>-0.09964296064043815</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -630,7 +630,7 @@
         <v>0</v>
       </c>
       <c r="J2">
-        <v>0.1254242036801028</v>
+        <v>0.04056893973315075</v>
       </c>
       <c r="K2" t="s">
         <v>49</v>
@@ -657,13 +657,13 @@
         <v>0</v>
       </c>
       <c r="S2">
-        <v>-1.277362294328371</v>
+        <v>-0.4131677333043157</v>
       </c>
       <c r="T2">
         <v>-0</v>
       </c>
       <c r="U2">
-        <v>1.277362294328371</v>
+        <v>0.4131677333043157</v>
       </c>
       <c r="V2">
         <v>1.672</v>
@@ -680,7 +680,7 @@
         <v>97.36</v>
       </c>
       <c r="C3">
-        <v>53.61318852835814</v>
+        <v>57.93416133347841</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -692,7 +692,7 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>-0.1827116754670441</v>
+        <v>0.1002380370831909</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -701,7 +701,7 @@
         <v>0</v>
       </c>
       <c r="J3">
-        <v>0.01509645522206494</v>
+        <v>0.1329921687846629</v>
       </c>
       <c r="K3" t="s">
         <v>49</v>
@@ -728,13 +728,13 @@
         <v>0</v>
       </c>
       <c r="S3">
-        <v>-0.155058085682672</v>
+        <v>-1.365983656374927</v>
       </c>
       <c r="T3">
         <v>-0</v>
       </c>
       <c r="U3">
-        <v>0.155058085682672</v>
+        <v>1.365983656374927</v>
       </c>
       <c r="V3">
         <v>1.874</v>
@@ -751,7 +751,7 @@
         <v>97.15000000000001</v>
       </c>
       <c r="C4">
-        <v>52.83789809994479</v>
+        <v>51.10424305160378</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -763,7 +763,7 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <v>0.1862493682020412</v>
+        <v>0.1447925793063786</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -772,7 +772,7 @@
         <v>0</v>
       </c>
       <c r="J4">
-        <v>0.1596470784175172</v>
+        <v>0.1423734163776577</v>
       </c>
       <c r="K4" t="s">
         <v>49</v>
@@ -799,13 +799,13 @@
         <v>0</v>
       </c>
       <c r="S4">
-        <v>-1.643304975990913</v>
+        <v>-1.465500940583199</v>
       </c>
       <c r="T4">
         <v>-0</v>
       </c>
       <c r="U4">
-        <v>1.643304975990913</v>
+        <v>1.465500940583199</v>
       </c>
       <c r="V4">
         <v>1.689</v>
@@ -822,7 +822,7 @@
         <v>96.66</v>
       </c>
       <c r="C5">
-        <v>44.62137321999023</v>
+        <v>43.77673834868779</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -834,7 +834,7 @@
         <v>0</v>
       </c>
       <c r="G5">
-        <v>-0.1348368821460769</v>
+        <v>-0.147203163018036</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -843,7 +843,7 @@
         <v>0</v>
       </c>
       <c r="J5">
-        <v>0.02336914577246795</v>
+        <v>0.01821652874248499</v>
       </c>
       <c r="K5" t="s">
         <v>49</v>
@@ -870,13 +870,13 @@
         <v>0</v>
       </c>
       <c r="S5">
-        <v>-0.2417664574019031</v>
+        <v>-0.1884598462909683</v>
       </c>
       <c r="T5">
         <v>-0</v>
       </c>
       <c r="U5">
-        <v>0.2417664574019031</v>
+        <v>0.1884598462909683</v>
       </c>
       <c r="V5">
         <v>1.646</v>
@@ -893,7 +893,7 @@
         <v>97.98</v>
       </c>
       <c r="C6">
-        <v>43.41254093298071</v>
+        <v>42.83443911723295</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -905,7 +905,7 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>0.07817142934729064</v>
+        <v>-0.06080966112291432</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -914,7 +914,7 @@
         <v>0</v>
       </c>
       <c r="J6">
-        <v>0.1273180888947044</v>
+        <v>0.06940930119878572</v>
       </c>
       <c r="K6" t="s">
         <v>49</v>
@@ -941,13 +941,13 @@
         <v>0</v>
       </c>
       <c r="S6">
-        <v>-1.29942936206067</v>
+        <v>-0.7084027474870964</v>
       </c>
       <c r="T6">
         <v>-0</v>
       </c>
       <c r="U6">
-        <v>1.29942936206067</v>
+        <v>0.7084027474870964</v>
       </c>
       <c r="V6">
         <v>1.934</v>
@@ -964,7 +964,7 @@
         <v>89.55</v>
       </c>
       <c r="C7">
-        <v>36.91539412267736</v>
+        <v>39.29242537979746</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -976,7 +976,7 @@
         <v>0</v>
       </c>
       <c r="G7">
-        <v>-0.1802439053241945</v>
+        <v>-0.1727246690462777</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -985,7 +985,7 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <v>0.002403897781585605</v>
+        <v>0.00553691289738429</v>
       </c>
       <c r="K7" t="s">
         <v>49</v>
@@ -1012,13 +1012,13 @@
         <v>0</v>
       </c>
       <c r="S7">
-        <v>-0.02684419633261424</v>
+        <v>-0.06183040644761909</v>
       </c>
       <c r="T7">
         <v>-0</v>
       </c>
       <c r="U7">
-        <v>0.02684419633261424</v>
+        <v>0.06183040644761909</v>
       </c>
       <c r="V7">
         <v>1.731</v>
@@ -1035,7 +1035,7 @@
         <v>104.21</v>
       </c>
       <c r="C8">
-        <v>36.78117314101429</v>
+        <v>38.98327334755937</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1047,7 +1047,7 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <v>0.1241296837367583</v>
+        <v>0.2427257399724055</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -1056,7 +1056,7 @@
         <v>0</v>
       </c>
       <c r="J8">
-        <v>0.1662995965569826</v>
+        <v>0.2157146199885023</v>
       </c>
       <c r="K8" t="s">
         <v>49</v>
@@ -1083,13 +1083,13 @@
         <v>0</v>
       </c>
       <c r="S8">
-        <v>-1.595812269043111</v>
+        <v>-2.069999232209023</v>
       </c>
       <c r="T8">
         <v>-0</v>
       </c>
       <c r="U8">
-        <v>1.595812269043111</v>
+        <v>2.069999232209023</v>
       </c>
       <c r="V8">
         <v>2.199</v>
@@ -1106,7 +1106,7 @@
         <v>118.21</v>
       </c>
       <c r="C9">
-        <v>28.80211179579874</v>
+        <v>28.63327718651425</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -1118,7 +1118,7 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <v>0.1830810567872892</v>
+        <v>0.1989264451110967</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -1127,7 +1127,7 @@
         <v>0</v>
       </c>
       <c r="J9">
-        <v>0.1724476086613705</v>
+        <v>0.1790498537962903</v>
       </c>
       <c r="K9" t="s">
         <v>49</v>
@@ -1154,13 +1154,13 @@
         <v>0</v>
       </c>
       <c r="S9">
-        <v>-1.178824199825484</v>
+        <v>-1.234676032453179</v>
       </c>
       <c r="T9">
         <v>-0.28</v>
       </c>
       <c r="U9">
-        <v>1.458824199825484</v>
+        <v>1.514676032453179</v>
       </c>
       <c r="V9">
         <v>1.627</v>
@@ -1177,7 +1177,7 @@
         <v>145</v>
       </c>
       <c r="C10">
-        <v>22.90799079667132</v>
+        <v>22.45989702424836</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -1189,7 +1189,7 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <v>0.2883546562410372</v>
+        <v>0.296465847503122</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -1198,7 +1198,7 @@
         <v>0</v>
       </c>
       <c r="J10">
-        <v>0.2457902734337655</v>
+        <v>0.2491699364596342</v>
       </c>
       <c r="K10" t="s">
         <v>49</v>
@@ -1225,13 +1225,13 @@
         <v>0</v>
       </c>
       <c r="S10">
-        <v>-0.4394053340259692</v>
+        <v>-0.462713354894029</v>
       </c>
       <c r="T10">
         <v>-1.2557</v>
       </c>
       <c r="U10">
-        <v>1.695105334025969</v>
+        <v>1.718413354894029</v>
       </c>
       <c r="V10">
         <v>1.733</v>
@@ -1248,28 +1248,28 @@
         <v>129.42</v>
       </c>
       <c r="C11">
-        <v>20.71096412654147</v>
+        <v>20.14633024977821</v>
       </c>
       <c r="D11">
-        <v>-0.07196041171828789</v>
+        <v>0.05363843590730929</v>
       </c>
       <c r="E11">
         <v>0.125</v>
       </c>
       <c r="F11">
-        <v>0.003598020585914395</v>
+        <v>0.002681921795365464</v>
       </c>
       <c r="G11">
-        <v>0.5137071692580222</v>
+        <v>0.5063040914611995</v>
       </c>
       <c r="H11">
-        <v>0.009313116484580818</v>
+        <v>0</v>
       </c>
       <c r="I11">
-        <v>-0.2077983794475419</v>
+        <v>-0.1945336894560735</v>
       </c>
       <c r="J11">
-        <v>0.2541016005524581</v>
+        <v>0.2604244041688025</v>
       </c>
       <c r="K11" t="s">
         <v>49</v>
@@ -1284,25 +1284,25 @@
         <v>0</v>
       </c>
       <c r="O11">
-        <v>0</v>
+        <v>0.05363843590730929</v>
       </c>
       <c r="P11">
         <v>0</v>
       </c>
       <c r="Q11">
-        <v>-1.605612574930783</v>
+        <v>-1.503119220028384</v>
       </c>
       <c r="R11">
-        <v>0.07196041171828789</v>
+        <v>0</v>
       </c>
       <c r="S11">
         <v>-0</v>
       </c>
       <c r="T11">
-        <v>-1.963387425069217</v>
+        <v>-2.012242344064306</v>
       </c>
       <c r="U11">
-        <v>1.963387425069217</v>
+        <v>2.012242344064306</v>
       </c>
       <c r="V11">
         <v>2.017</v>
@@ -1319,28 +1319,28 @@
         <v>100.82</v>
       </c>
       <c r="C12">
-        <v>20.35116206795003</v>
+        <v>20.41452242931476</v>
       </c>
       <c r="D12">
-        <v>9.569292922643363</v>
+        <v>-0.08290448586295129</v>
       </c>
       <c r="E12">
         <v>0.125</v>
       </c>
       <c r="F12">
-        <v>0.4784646461321682</v>
+        <v>0.004145224293147565</v>
       </c>
       <c r="G12">
-        <v>-0.531409061546366</v>
+        <v>0.5828460436691346</v>
       </c>
       <c r="H12">
-        <v>0</v>
+        <v>0.008358430264702749</v>
       </c>
       <c r="I12">
-        <v>0</v>
+        <v>-0.3475300475682628</v>
       </c>
       <c r="J12">
-        <v>0.1756689378389321</v>
+        <v>0.1903950624317371</v>
       </c>
       <c r="K12" t="s">
         <v>49</v>
@@ -1355,25 +1355,25 @@
         <v>0</v>
       </c>
       <c r="O12">
-        <v>3.5930983154242</v>
+        <v>0</v>
       </c>
       <c r="P12">
-        <v>5.976194607219163</v>
+        <v>0</v>
       </c>
       <c r="Q12">
-        <v>0</v>
+        <v>-3.447034790401338</v>
       </c>
       <c r="R12">
-        <v>0</v>
+        <v>0.08290448586295129</v>
       </c>
       <c r="S12">
         <v>-0</v>
       </c>
       <c r="T12">
-        <v>-1.7424016845758</v>
+        <v>-1.888465209598662</v>
       </c>
       <c r="U12">
-        <v>1.7424016845758</v>
+        <v>1.888465209598662</v>
       </c>
       <c r="V12">
         <v>1.901</v>
@@ -1390,28 +1390,28 @@
         <v>94.12</v>
       </c>
       <c r="C13">
-        <v>68.19762668116684</v>
+        <v>20</v>
       </c>
       <c r="D13">
-        <v>4.360474663766631</v>
+        <v>0.0665026364182492</v>
       </c>
       <c r="E13">
         <v>0.125</v>
       </c>
       <c r="F13">
-        <v>0.2180237331883315</v>
+        <v>0.00332513182091246</v>
       </c>
       <c r="G13">
-        <v>0.1504641956308077</v>
+        <v>0.5667609137338332</v>
       </c>
       <c r="H13">
         <v>0</v>
       </c>
       <c r="I13">
-        <v>0</v>
+        <v>-0.3517176670935154</v>
       </c>
       <c r="J13">
-        <v>0.178006937046055</v>
+        <v>0.1793918327667991</v>
       </c>
       <c r="K13" t="s">
         <v>49</v>
@@ -1426,13 +1426,13 @@
         <v>0</v>
       </c>
       <c r="O13">
-        <v>3.818123575796271</v>
+        <v>0.0665026364182492</v>
       </c>
       <c r="P13">
-        <v>0.5423510879703599</v>
+        <v>0</v>
       </c>
       <c r="Q13">
-        <v>0</v>
+        <v>-3.736906790198846</v>
       </c>
       <c r="R13">
         <v>0</v>
@@ -1441,10 +1441,10 @@
         <v>-0</v>
       </c>
       <c r="T13">
-        <v>-1.891276424203729</v>
+        <v>-1.905990573382905</v>
       </c>
       <c r="U13">
-        <v>1.891276424203729</v>
+        <v>1.905990573382905</v>
       </c>
       <c r="V13">
         <v>1.908</v>
@@ -1461,28 +1461,28 @@
         <v>82.59999999999999</v>
       </c>
       <c r="C14">
-        <v>90</v>
+        <v>20.33251318209125</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>9.568951284978123</v>
       </c>
       <c r="E14">
         <v>0.125</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>0.4784475642489062</v>
       </c>
       <c r="G14">
-        <v>0.6075800284124606</v>
+        <v>-0.2552119646574454</v>
       </c>
       <c r="H14">
         <v>0</v>
       </c>
       <c r="I14">
-        <v>-0.4373781854196709</v>
+        <v>0</v>
       </c>
       <c r="J14">
-        <v>0.142242534580329</v>
+        <v>0.1407482189246551</v>
       </c>
       <c r="K14" t="s">
         <v>49</v>
@@ -1497,13 +1497,13 @@
         <v>0</v>
       </c>
       <c r="O14">
-        <v>0</v>
+        <v>5.31322640527052</v>
       </c>
       <c r="P14">
-        <v>0</v>
+        <v>4.255724879707603</v>
       </c>
       <c r="Q14">
-        <v>-5.295135416703038</v>
+        <v>0</v>
       </c>
       <c r="R14">
         <v>0</v>
@@ -1512,10 +1512,10 @@
         <v>-0</v>
       </c>
       <c r="T14">
-        <v>-1.722064583296962</v>
+        <v>-1.70397359472948</v>
       </c>
       <c r="U14">
-        <v>1.722064583296962</v>
+        <v>1.70397359472948</v>
       </c>
       <c r="V14">
         <v>1.727</v>
@@ -1532,28 +1532,28 @@
         <v>85.59999999999999</v>
       </c>
       <c r="C15">
-        <v>90</v>
+        <v>68.17726960698187</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>4.350197306749376</v>
       </c>
       <c r="E15">
         <v>0.125</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>0.2175098653374688</v>
       </c>
       <c r="G15">
-        <v>0.6986772554757278</v>
+        <v>0.3264098445010066</v>
       </c>
       <c r="H15">
         <v>0</v>
       </c>
       <c r="I15">
-        <v>-0.5017457775173373</v>
+        <v>-0.1292906891431441</v>
       </c>
       <c r="J15">
-        <v>0.1643163824826627</v>
+        <v>0.1643945813991094</v>
       </c>
       <c r="K15" t="s">
         <v>49</v>
@@ -1568,13 +1568,13 @@
         <v>0</v>
       </c>
       <c r="O15">
-        <v>0</v>
+        <v>4.350197306749376</v>
       </c>
       <c r="P15">
         <v>0</v>
       </c>
       <c r="Q15">
-        <v>-5.861516092492258</v>
+        <v>-1.510405246999347</v>
       </c>
       <c r="R15">
         <v>0</v>
@@ -1583,10 +1583,10 @@
         <v>-0</v>
       </c>
       <c r="T15">
-        <v>-1.919583907507742</v>
+        <v>-1.920497446251278</v>
       </c>
       <c r="U15">
-        <v>1.919583907507742</v>
+        <v>1.920497446251278</v>
       </c>
       <c r="V15">
         <v>1.922</v>
@@ -1603,28 +1603,28 @@
         <v>94.2</v>
       </c>
       <c r="C16">
-        <v>90</v>
+        <v>89.92825614072875</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>0.01434877185425121</v>
       </c>
       <c r="E16">
         <v>0.125</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>0.0007174385927125604</v>
       </c>
       <c r="G16">
-        <v>0.7520363545585835</v>
+        <v>0.7509851717917728</v>
       </c>
       <c r="H16">
         <v>0</v>
       </c>
       <c r="I16">
-        <v>-0.5615638267438692</v>
+        <v>-0.5599975499052988</v>
       </c>
       <c r="J16">
-        <v>0.159009653256131</v>
+        <v>0.1592242757860308</v>
       </c>
       <c r="K16" t="s">
         <v>49</v>
@@ -1639,13 +1639,13 @@
         <v>0</v>
       </c>
       <c r="O16">
-        <v>0</v>
+        <v>0.01434877185425121</v>
       </c>
       <c r="P16">
         <v>0</v>
       </c>
       <c r="Q16">
-        <v>-5.961399434648293</v>
+        <v>-5.944772291988309</v>
       </c>
       <c r="R16">
         <v>0</v>
@@ -1654,10 +1654,10 @@
         <v>-0</v>
       </c>
       <c r="T16">
-        <v>-1.688000565351709</v>
+        <v>-1.69027893615744</v>
       </c>
       <c r="U16">
-        <v>1.688000565351709</v>
+        <v>1.69027893615744</v>
       </c>
       <c r="V16">
         <v>1.691</v>
@@ -1686,16 +1686,16 @@
         <v>0</v>
       </c>
       <c r="G17">
-        <v>0.6987856516612041</v>
+        <v>0.7036673816309533</v>
       </c>
       <c r="H17">
         <v>0</v>
       </c>
       <c r="I17">
-        <v>-0.4825702488134256</v>
+        <v>-0.4790832988350333</v>
       </c>
       <c r="J17">
-        <v>0.1841397511865744</v>
+        <v>0.1876267011649667</v>
       </c>
       <c r="K17" t="s">
         <v>49</v>
@@ -1716,7 +1716,7 @@
         <v>0</v>
       </c>
       <c r="Q17">
-        <v>-5.079686829615007</v>
+        <v>-5.042982093000351</v>
       </c>
       <c r="R17">
         <v>0</v>
@@ -1725,10 +1725,10 @@
         <v>-0</v>
       </c>
       <c r="T17">
-        <v>-1.938313170384993</v>
+        <v>-1.975017906999649</v>
       </c>
       <c r="U17">
-        <v>1.938313170384993</v>
+        <v>1.975017906999649</v>
       </c>
       <c r="V17">
         <v>1.98</v>
@@ -1757,16 +1757,16 @@
         <v>0</v>
       </c>
       <c r="G18">
-        <v>0.6084620924954033</v>
+        <v>0.6133189994537185</v>
       </c>
       <c r="H18">
         <v>0</v>
       </c>
       <c r="I18">
-        <v>-0.3944134596461407</v>
+        <v>-0.3909442403902012</v>
       </c>
       <c r="J18">
-        <v>0.1839389303538594</v>
+        <v>0.1874081496097989</v>
       </c>
       <c r="K18" t="s">
         <v>49</v>
@@ -1787,7 +1787,7 @@
         <v>0</v>
       </c>
       <c r="Q18">
-        <v>-3.996083684358061</v>
+        <v>-3.960934553092211</v>
       </c>
       <c r="R18">
         <v>0</v>
@@ -1796,10 +1796,10 @@
         <v>-0</v>
       </c>
       <c r="T18">
-        <v>-1.86361631564194</v>
+        <v>-1.89876544690779</v>
       </c>
       <c r="U18">
-        <v>1.86361631564194</v>
+        <v>1.89876544690779</v>
       </c>
       <c r="V18">
         <v>1.92</v>
@@ -1828,16 +1828,16 @@
         <v>0</v>
       </c>
       <c r="G19">
-        <v>0.4675429995750385</v>
+        <v>0.4709918912341285</v>
       </c>
       <c r="H19">
         <v>0</v>
       </c>
       <c r="I19">
-        <v>-0.2656832860178297</v>
+        <v>-0.2632197919756225</v>
       </c>
       <c r="J19">
-        <v>0.1720532139821703</v>
+        <v>0.1745167080243775</v>
       </c>
       <c r="K19" t="s">
         <v>49</v>
@@ -1858,7 +1858,7 @@
         <v>0</v>
       </c>
       <c r="Q19">
-        <v>-2.592032058710533</v>
+        <v>-2.567997970493878</v>
       </c>
       <c r="R19">
         <v>0</v>
@@ -1867,10 +1867,10 @@
         <v>-0</v>
       </c>
       <c r="T19">
-        <v>-1.678567941289467</v>
+        <v>-1.702602029506122</v>
       </c>
       <c r="U19">
-        <v>1.678567941289467</v>
+        <v>1.702602029506122</v>
       </c>
       <c r="V19">
         <v>1.716</v>
@@ -1899,16 +1899,16 @@
         <v>0</v>
       </c>
       <c r="G20">
-        <v>0.2872120041056374</v>
+        <v>0.2974855427783252</v>
       </c>
       <c r="H20">
         <v>0</v>
       </c>
       <c r="I20">
-        <v>-0.04777718678168758</v>
+        <v>-0.04043894487262485</v>
       </c>
       <c r="J20">
-        <v>0.2073548572183125</v>
+        <v>0.2146930991273752</v>
       </c>
       <c r="K20" t="s">
         <v>49</v>
@@ -1929,7 +1929,7 @@
         <v>0</v>
       </c>
       <c r="Q20">
-        <v>-0.4429555607425142</v>
+        <v>-0.3749206830393552</v>
       </c>
       <c r="R20">
         <v>0</v>
@@ -1938,10 +1938,10 @@
         <v>-0</v>
       </c>
       <c r="T20">
-        <v>-1.922444439257486</v>
+        <v>-1.990479316960645</v>
       </c>
       <c r="U20">
-        <v>1.922444439257486</v>
+        <v>1.990479316960645</v>
       </c>
       <c r="V20">
         <v>1.995</v>
@@ -1961,25 +1961,25 @@
         <v>90</v>
       </c>
       <c r="D21">
-        <v>-3.545230081427158</v>
+        <v>0</v>
       </c>
       <c r="E21">
         <v>0.125</v>
       </c>
       <c r="F21">
-        <v>0.1772615040713579</v>
+        <v>0</v>
       </c>
       <c r="G21">
-        <v>0.8038167527326658</v>
+        <v>0.2865811706973438</v>
       </c>
       <c r="H21">
-        <v>0.5353297422955008</v>
+        <v>0</v>
       </c>
       <c r="I21">
         <v>0</v>
       </c>
       <c r="J21">
-        <v>0.2316125876821521</v>
+        <v>0.2391518211238932</v>
       </c>
       <c r="K21" t="s">
         <v>49</v>
@@ -2003,16 +2003,16 @@
         <v>0</v>
       </c>
       <c r="R21">
-        <v>3.545230081427158</v>
+        <v>0</v>
       </c>
       <c r="S21">
-        <v>-0.9948581965705438</v>
+        <v>-1.04478689486022</v>
       </c>
       <c r="T21">
         <v>-0.539</v>
       </c>
       <c r="U21">
-        <v>1.533858196570544</v>
+        <v>1.58378689486022</v>
       </c>
       <c r="V21">
         <v>1.586</v>
@@ -2029,28 +2029,28 @@
         <v>149.85</v>
       </c>
       <c r="C22">
-        <v>67.29955861001149</v>
+        <v>84.7760655256989</v>
       </c>
       <c r="D22">
-        <v>-0.6356641860938619</v>
+        <v>-3.973845061920404</v>
       </c>
       <c r="E22">
         <v>0.125</v>
       </c>
       <c r="F22">
-        <v>0.0317832093046931</v>
+        <v>0.1986922530960202</v>
       </c>
       <c r="G22">
-        <v>0.4471488922102323</v>
+        <v>0.9568295182350837</v>
       </c>
       <c r="H22">
-        <v>0.0952542782861652</v>
+        <v>0.5954806825287726</v>
       </c>
       <c r="I22">
         <v>0</v>
       </c>
       <c r="J22">
-        <v>0.2995446808016946</v>
+        <v>0.3034839398776296</v>
       </c>
       <c r="K22" t="s">
         <v>49</v>
@@ -2074,16 +2074,16 @@
         <v>0</v>
       </c>
       <c r="R22">
-        <v>0.6356641860938619</v>
+        <v>3.973845061920404</v>
       </c>
       <c r="S22">
-        <v>-1.861763502180144</v>
+        <v>-1.888051517368232</v>
       </c>
       <c r="T22">
         <v>-0.1372</v>
       </c>
       <c r="U22">
-        <v>1.998963502180144</v>
+        <v>2.025251517368232</v>
       </c>
       <c r="V22">
         <v>2.041</v>
@@ -2100,7 +2100,7 @@
         <v>133.8</v>
       </c>
       <c r="C23">
-        <v>54.81242016864146</v>
+        <v>55.46658262925571</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -2112,7 +2112,7 @@
         <v>0</v>
       </c>
       <c r="G23">
-        <v>0.3087873626561608</v>
+        <v>0.3132436138822211</v>
       </c>
       <c r="H23">
         <v>0</v>
@@ -2121,7 +2121,7 @@
         <v>0</v>
       </c>
       <c r="J23">
-        <v>0.2600530011067337</v>
+        <v>0.2619097724509254</v>
       </c>
       <c r="K23" t="s">
         <v>49</v>
@@ -2148,13 +2148,13 @@
         <v>0</v>
       </c>
       <c r="S23">
-        <v>-1.943594926059295</v>
+        <v>-1.95747214088883</v>
       </c>
       <c r="T23">
         <v>-0</v>
       </c>
       <c r="U23">
-        <v>1.943594926059295</v>
+        <v>1.95747214088883</v>
       </c>
       <c r="V23">
         <v>1.964</v>
@@ -2171,7 +2171,7 @@
         <v>103.85</v>
       </c>
       <c r="C24">
-        <v>45.09444553834498</v>
+        <v>45.67922192481156</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -2183,7 +2183,7 @@
         <v>0</v>
       </c>
       <c r="G24">
-        <v>0.1807805915539906</v>
+        <v>0.2261639410261073</v>
       </c>
       <c r="H24">
         <v>0</v>
@@ -2192,7 +2192,7 @@
         <v>0</v>
       </c>
       <c r="J24">
-        <v>0.1716980464808294</v>
+        <v>0.1906077754275447</v>
       </c>
       <c r="K24" t="s">
         <v>49</v>
@@ -2219,13 +2219,13 @@
         <v>0</v>
       </c>
       <c r="S24">
-        <v>-1.653327361394602</v>
+        <v>-1.835414303587335</v>
       </c>
       <c r="T24">
         <v>-0</v>
       </c>
       <c r="U24">
-        <v>1.653327361394602</v>
+        <v>1.835414303587335</v>
       </c>
       <c r="V24">
         <v>1.856</v>
@@ -2242,7 +2242,7 @@
         <v>96</v>
       </c>
       <c r="C25">
-        <v>36.82780873137197</v>
+        <v>36.50215040687489</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -2254,7 +2254,7 @@
         <v>0</v>
       </c>
       <c r="G25">
-        <v>0.188959604518682</v>
+        <v>0.1831422753691164</v>
       </c>
       <c r="H25">
         <v>0</v>
@@ -2263,7 +2263,7 @@
         <v>0</v>
       </c>
       <c r="J25">
-        <v>0.1597571685494508</v>
+        <v>0.1573332814037985</v>
       </c>
       <c r="K25" t="s">
         <v>49</v>
@@ -2290,13 +2290,13 @@
         <v>0</v>
       </c>
       <c r="S25">
-        <v>-1.664137172390113</v>
+        <v>-1.638888347956234</v>
       </c>
       <c r="T25">
         <v>-0</v>
       </c>
       <c r="U25">
-        <v>1.664137172390113</v>
+        <v>1.638888347956234</v>
       </c>
       <c r="V25">
         <v>1.688</v>
@@ -2313,28 +2313,28 @@
         <v>102.95</v>
       </c>
       <c r="C26">
-        <v>28.50712286942141</v>
+        <v>28.30770866709372</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>-0.008479629924323051</v>
       </c>
       <c r="E26">
         <v>0.125</v>
       </c>
       <c r="F26">
-        <v>0</v>
+        <v>0.0004239814962161526</v>
       </c>
       <c r="G26">
-        <v>0.197632972444981</v>
+        <v>0.2042351624321104</v>
       </c>
       <c r="H26">
-        <v>0</v>
+        <v>0.0008729779007090582</v>
       </c>
       <c r="I26">
         <v>0</v>
       </c>
       <c r="J26">
-        <v>0.1677955718520754</v>
+        <v>0.1701827435547506</v>
       </c>
       <c r="K26" t="s">
         <v>49</v>
@@ -2358,16 +2358,16 @@
         <v>0</v>
       </c>
       <c r="R26">
-        <v>0</v>
+        <v>0.008479629924323051</v>
       </c>
       <c r="S26">
-        <v>-1.629874423041043</v>
+        <v>-1.65306210349442</v>
       </c>
       <c r="T26">
         <v>-0</v>
       </c>
       <c r="U26">
-        <v>1.629874423041043</v>
+        <v>1.65306210349442</v>
       </c>
       <c r="V26">
         <v>1.66</v>
@@ -2384,7 +2384,7 @@
         <v>100.85</v>
       </c>
       <c r="C27">
-        <v>20.35775075421619</v>
+        <v>20</v>
       </c>
       <c r="D27">
         <v>0</v>

</xml_diff>

<commit_message>
Trying to fix code damn
</commit_message>
<xml_diff>
--- a/data/Output/xlsx/results.xlsx
+++ b/data/Output/xlsx/results.xlsx
@@ -621,7 +621,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>-0.09964296064043815</v>
+        <v>0.1294427768909185</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -630,7 +630,7 @@
         <v>0</v>
       </c>
       <c r="J2">
-        <v>0.04056893973315075</v>
+        <v>0.136021330371216</v>
       </c>
       <c r="K2" t="s">
         <v>49</v>
@@ -657,13 +657,13 @@
         <v>0</v>
       </c>
       <c r="S2">
-        <v>-0.4131677333043157</v>
+        <v>-1.385286998382891</v>
       </c>
       <c r="T2">
         <v>-0</v>
       </c>
       <c r="U2">
-        <v>0.4131677333043157</v>
+        <v>1.385286998382891</v>
       </c>
       <c r="V2">
         <v>1.672</v>
@@ -680,7 +680,7 @@
         <v>97.36</v>
       </c>
       <c r="C3">
-        <v>57.93416133347841</v>
+        <v>53.07356500808555</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -692,7 +692,7 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0.1002380370831909</v>
+        <v>0.1839686096833563</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -701,7 +701,7 @@
         <v>0</v>
       </c>
       <c r="J3">
-        <v>0.1329921687846629</v>
+        <v>0.1678799073680652</v>
       </c>
       <c r="K3" t="s">
         <v>49</v>
@@ -728,13 +728,13 @@
         <v>0</v>
       </c>
       <c r="S3">
-        <v>-1.365983656374927</v>
+        <v>-1.724321152095986</v>
       </c>
       <c r="T3">
         <v>-0</v>
       </c>
       <c r="U3">
-        <v>1.365983656374927</v>
+        <v>1.724321152095986</v>
       </c>
       <c r="V3">
         <v>1.874</v>
@@ -751,7 +751,7 @@
         <v>97.15000000000001</v>
       </c>
       <c r="C4">
-        <v>51.10424305160378</v>
+        <v>44.45195924760561</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -763,7 +763,7 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <v>0.1447925793063786</v>
+        <v>0.1960820334845552</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -772,7 +772,7 @@
         <v>0</v>
       </c>
       <c r="J4">
-        <v>0.1423734163776577</v>
+        <v>0.1637440222852313</v>
       </c>
       <c r="K4" t="s">
         <v>49</v>
@@ -799,13 +799,13 @@
         <v>0</v>
       </c>
       <c r="S4">
-        <v>-1.465500940583199</v>
+        <v>-1.685476297326107</v>
       </c>
       <c r="T4">
         <v>-0</v>
       </c>
       <c r="U4">
-        <v>1.465500940583199</v>
+        <v>1.685476297326107</v>
       </c>
       <c r="V4">
         <v>1.689</v>
@@ -822,7 +822,7 @@
         <v>96.66</v>
       </c>
       <c r="C5">
-        <v>43.77673834868779</v>
+        <v>36.02457776097508</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -834,7 +834,7 @@
         <v>0</v>
       </c>
       <c r="G5">
-        <v>-0.147203163018036</v>
+        <v>0.1425237157371368</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -843,7 +843,7 @@
         <v>0</v>
       </c>
       <c r="J5">
-        <v>0.01821652874248499</v>
+        <v>0.1389360615571403</v>
       </c>
       <c r="K5" t="s">
         <v>49</v>
@@ -870,13 +870,13 @@
         <v>0</v>
       </c>
       <c r="S5">
-        <v>-0.1884598462909683</v>
+        <v>-1.437368731193258</v>
       </c>
       <c r="T5">
         <v>-0</v>
       </c>
       <c r="U5">
-        <v>0.1884598462909683</v>
+        <v>1.437368731193258</v>
       </c>
       <c r="V5">
         <v>1.646</v>
@@ -893,28 +893,28 @@
         <v>97.98</v>
       </c>
       <c r="C6">
-        <v>42.83443911723295</v>
+        <v>28.83773410500879</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>-0.02066547782790784</v>
       </c>
       <c r="E6">
         <v>0.125</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>0.001033273891395392</v>
       </c>
       <c r="G6">
-        <v>-0.06080966112291432</v>
+        <v>0.1854154611275955</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>0.00202480351757841</v>
       </c>
       <c r="I6">
         <v>0</v>
       </c>
       <c r="J6">
-        <v>0.06940930119878572</v>
+        <v>0.1711594340041738</v>
       </c>
       <c r="K6" t="s">
         <v>49</v>
@@ -938,16 +938,16 @@
         <v>0</v>
       </c>
       <c r="R6">
-        <v>0</v>
+        <v>0.02066547782790784</v>
       </c>
       <c r="S6">
-        <v>-0.7084027474870964</v>
+        <v>-1.74688134317385</v>
       </c>
       <c r="T6">
         <v>-0</v>
       </c>
       <c r="U6">
-        <v>0.7084027474870964</v>
+        <v>1.74688134317385</v>
       </c>
       <c r="V6">
         <v>1.934</v>
@@ -964,19 +964,19 @@
         <v>89.55</v>
       </c>
       <c r="C7">
-        <v>39.29242537979746</v>
+        <v>20</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>9.570888597260158</v>
       </c>
       <c r="E7">
         <v>0.125</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>0.4785444298630079</v>
       </c>
       <c r="G7">
-        <v>-0.1727246690462777</v>
+        <v>-1.214500948661576</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -985,7 +985,7 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <v>0.00553691289738429</v>
+        <v>0</v>
       </c>
       <c r="K7" t="s">
         <v>49</v>
@@ -1003,7 +1003,7 @@
         <v>0</v>
       </c>
       <c r="P7">
-        <v>0</v>
+        <v>9.570888597260158</v>
       </c>
       <c r="Q7">
         <v>0</v>
@@ -1012,13 +1012,13 @@
         <v>0</v>
       </c>
       <c r="S7">
-        <v>-0.06183040644761909</v>
+        <v>-0</v>
       </c>
       <c r="T7">
         <v>-0</v>
       </c>
       <c r="U7">
-        <v>0.06183040644761909</v>
+        <v>0</v>
       </c>
       <c r="V7">
         <v>1.731</v>
@@ -1035,7 +1035,7 @@
         <v>104.21</v>
       </c>
       <c r="C8">
-        <v>38.98327334755937</v>
+        <v>67.8544429863008</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1047,7 +1047,7 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <v>0.2427257399724055</v>
+        <v>0.09576465376964684</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -1056,7 +1056,7 @@
         <v>0</v>
       </c>
       <c r="J8">
-        <v>0.2157146199885023</v>
+        <v>0.1544808340706862</v>
       </c>
       <c r="K8" t="s">
         <v>49</v>
@@ -1083,13 +1083,13 @@
         <v>0</v>
       </c>
       <c r="S8">
-        <v>-2.069999232209023</v>
+        <v>-1.482399328957741</v>
       </c>
       <c r="T8">
         <v>-0</v>
       </c>
       <c r="U8">
-        <v>2.069999232209023</v>
+        <v>1.482399328957741</v>
       </c>
       <c r="V8">
         <v>2.199</v>
@@ -1106,7 +1106,7 @@
         <v>118.21</v>
       </c>
       <c r="C9">
-        <v>28.63327718651425</v>
+        <v>60.44244634151208</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -1118,7 +1118,7 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <v>0.1989264451110967</v>
+        <v>0.1840019904277628</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -1127,7 +1127,7 @@
         <v>0</v>
       </c>
       <c r="J9">
-        <v>0.1790498537962903</v>
+        <v>0.1728313310115678</v>
       </c>
       <c r="K9" t="s">
         <v>49</v>
@@ -1154,19 +1154,19 @@
         <v>0</v>
       </c>
       <c r="S9">
-        <v>-1.234676032453179</v>
+        <v>-1.462070307178478</v>
       </c>
       <c r="T9">
-        <v>-0.28</v>
+        <v>-0</v>
       </c>
       <c r="U9">
-        <v>1.514676032453179</v>
+        <v>1.462070307178478</v>
       </c>
       <c r="V9">
         <v>1.627</v>
       </c>
       <c r="W9">
-        <v>0.28</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:23">
@@ -1177,7 +1177,7 @@
         <v>145</v>
       </c>
       <c r="C10">
-        <v>22.45989702424836</v>
+        <v>53.13209480561969</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -1189,7 +1189,7 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <v>0.296465847503122</v>
+        <v>0.2625408050941181</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -1198,7 +1198,7 @@
         <v>0</v>
       </c>
       <c r="J10">
-        <v>0.2491699364596342</v>
+        <v>0.2350345021225493</v>
       </c>
       <c r="K10" t="s">
         <v>49</v>
@@ -1225,19 +1225,19 @@
         <v>0</v>
       </c>
       <c r="S10">
-        <v>-0.462713354894029</v>
+        <v>-1.620927600845167</v>
       </c>
       <c r="T10">
-        <v>-1.2557</v>
+        <v>-0</v>
       </c>
       <c r="U10">
-        <v>1.718413354894029</v>
+        <v>1.620927600845167</v>
       </c>
       <c r="V10">
         <v>1.733</v>
       </c>
       <c r="W10">
-        <v>1.2557</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:23">
@@ -1248,28 +1248,28 @@
         <v>129.42</v>
       </c>
       <c r="C11">
-        <v>20.14633024977821</v>
+        <v>45.02745680139385</v>
       </c>
       <c r="D11">
-        <v>0.05363843590730929</v>
+        <v>0</v>
       </c>
       <c r="E11">
         <v>0.125</v>
       </c>
       <c r="F11">
-        <v>0.002681921795365464</v>
+        <v>0</v>
       </c>
       <c r="G11">
-        <v>0.5063040914611995</v>
+        <v>0.2899672715031826</v>
       </c>
       <c r="H11">
         <v>0</v>
       </c>
       <c r="I11">
-        <v>-0.1945336894560735</v>
+        <v>0</v>
       </c>
       <c r="J11">
-        <v>0.2604244041688025</v>
+        <v>0.2513397664596594</v>
       </c>
       <c r="K11" t="s">
         <v>49</v>
@@ -1284,31 +1284,31 @@
         <v>0</v>
       </c>
       <c r="O11">
-        <v>0.05363843590730929</v>
+        <v>0</v>
       </c>
       <c r="P11">
         <v>0</v>
       </c>
       <c r="Q11">
-        <v>-1.503119220028384</v>
+        <v>0</v>
       </c>
       <c r="R11">
         <v>0</v>
       </c>
       <c r="S11">
-        <v>-0</v>
+        <v>-1.942047337812235</v>
       </c>
       <c r="T11">
-        <v>-2.012242344064306</v>
+        <v>-0</v>
       </c>
       <c r="U11">
-        <v>2.012242344064306</v>
+        <v>1.942047337812235</v>
       </c>
       <c r="V11">
         <v>2.017</v>
       </c>
       <c r="W11">
-        <v>3.569</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:23">
@@ -1319,28 +1319,28 @@
         <v>100.82</v>
       </c>
       <c r="C12">
-        <v>20.41452242931476</v>
+        <v>35.31722011233268</v>
       </c>
       <c r="D12">
-        <v>-0.08290448586295129</v>
+        <v>0</v>
       </c>
       <c r="E12">
         <v>0.125</v>
       </c>
       <c r="F12">
-        <v>0.004145224293147565</v>
+        <v>0</v>
       </c>
       <c r="G12">
-        <v>0.5828460436691346</v>
+        <v>0.226580851315367</v>
       </c>
       <c r="H12">
-        <v>0.008358430264702749</v>
+        <v>0</v>
       </c>
       <c r="I12">
-        <v>-0.3475300475682628</v>
+        <v>0</v>
       </c>
       <c r="J12">
-        <v>0.1903950624317371</v>
+        <v>0.1902380980480696</v>
       </c>
       <c r="K12" t="s">
         <v>49</v>
@@ -1361,25 +1361,25 @@
         <v>0</v>
       </c>
       <c r="Q12">
-        <v>-3.447034790401338</v>
+        <v>0</v>
       </c>
       <c r="R12">
-        <v>0.08290448586295129</v>
+        <v>0</v>
       </c>
       <c r="S12">
-        <v>-0</v>
+        <v>-1.886908332157008</v>
       </c>
       <c r="T12">
-        <v>-1.888465209598662</v>
+        <v>-0</v>
       </c>
       <c r="U12">
-        <v>1.888465209598662</v>
+        <v>1.886908332157008</v>
       </c>
       <c r="V12">
         <v>1.901</v>
       </c>
       <c r="W12">
-        <v>5.3355</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:23">
@@ -1390,28 +1390,28 @@
         <v>94.12</v>
       </c>
       <c r="C13">
-        <v>20</v>
+        <v>25.88267845154764</v>
       </c>
       <c r="D13">
-        <v>0.0665026364182492</v>
+        <v>-0.04914236872111433</v>
       </c>
       <c r="E13">
         <v>0.125</v>
       </c>
       <c r="F13">
-        <v>0.00332513182091246</v>
+        <v>0.002457118436055716</v>
       </c>
       <c r="G13">
-        <v>0.5667609137338332</v>
+        <v>0.04379275037099467</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>0.004625279744031281</v>
       </c>
       <c r="I13">
-        <v>-0.3517176670935154</v>
+        <v>0</v>
       </c>
       <c r="J13">
-        <v>0.1793918327667991</v>
+        <v>0.1061102594279014</v>
       </c>
       <c r="K13" t="s">
         <v>49</v>
@@ -1426,31 +1426,31 @@
         <v>0</v>
       </c>
       <c r="O13">
-        <v>0.0665026364182492</v>
+        <v>0</v>
       </c>
       <c r="P13">
         <v>0</v>
       </c>
       <c r="Q13">
-        <v>-3.736906790198846</v>
+        <v>0</v>
       </c>
       <c r="R13">
-        <v>0</v>
+        <v>0.04914236872111433</v>
       </c>
       <c r="S13">
-        <v>-0</v>
+        <v>-1.127393321588413</v>
       </c>
       <c r="T13">
-        <v>-1.905990573382905</v>
+        <v>-0</v>
       </c>
       <c r="U13">
-        <v>1.905990573382905</v>
+        <v>1.127393321588413</v>
       </c>
       <c r="V13">
         <v>1.908</v>
       </c>
       <c r="W13">
-        <v>5.7094</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:23">
@@ -1461,19 +1461,19 @@
         <v>82.59999999999999</v>
       </c>
       <c r="C14">
-        <v>20.33251318209125</v>
+        <v>20</v>
       </c>
       <c r="D14">
-        <v>9.568951284978123</v>
+        <v>3.217214041083077</v>
       </c>
       <c r="E14">
         <v>0.125</v>
       </c>
       <c r="F14">
-        <v>0.4784475642489062</v>
+        <v>0.1608607020541538</v>
       </c>
       <c r="G14">
-        <v>-0.2552119646574454</v>
+        <v>-0.4900704957521546</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -1482,7 +1482,7 @@
         <v>0</v>
       </c>
       <c r="J14">
-        <v>0.1407482189246551</v>
+        <v>0</v>
       </c>
       <c r="K14" t="s">
         <v>49</v>
@@ -1497,10 +1497,10 @@
         <v>0</v>
       </c>
       <c r="O14">
-        <v>5.31322640527052</v>
+        <v>0</v>
       </c>
       <c r="P14">
-        <v>4.255724879707603</v>
+        <v>3.217214041083077</v>
       </c>
       <c r="Q14">
         <v>0</v>
@@ -1512,16 +1512,16 @@
         <v>-0</v>
       </c>
       <c r="T14">
-        <v>-1.70397359472948</v>
+        <v>-0</v>
       </c>
       <c r="U14">
-        <v>1.70397359472948</v>
+        <v>0</v>
       </c>
       <c r="V14">
         <v>1.727</v>
       </c>
       <c r="W14">
-        <v>7.017200000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:23">
@@ -1532,28 +1532,28 @@
         <v>85.59999999999999</v>
       </c>
       <c r="C15">
-        <v>68.17726960698187</v>
+        <v>36.08607020541539</v>
       </c>
       <c r="D15">
-        <v>4.350197306749376</v>
+        <v>0</v>
       </c>
       <c r="E15">
         <v>0.125</v>
       </c>
       <c r="F15">
-        <v>0.2175098653374688</v>
+        <v>0</v>
       </c>
       <c r="G15">
-        <v>0.3264098445010066</v>
+        <v>0.1047120477578028</v>
       </c>
       <c r="H15">
         <v>0</v>
       </c>
       <c r="I15">
-        <v>-0.1292906891431441</v>
+        <v>0</v>
       </c>
       <c r="J15">
-        <v>0.1643945813991094</v>
+        <v>0.1258916198990845</v>
       </c>
       <c r="K15" t="s">
         <v>49</v>
@@ -1568,31 +1568,31 @@
         <v>0</v>
       </c>
       <c r="O15">
-        <v>4.350197306749376</v>
+        <v>0</v>
       </c>
       <c r="P15">
         <v>0</v>
       </c>
       <c r="Q15">
-        <v>-1.510405246999347</v>
+        <v>0</v>
       </c>
       <c r="R15">
         <v>0</v>
       </c>
       <c r="S15">
-        <v>-0</v>
+        <v>-1.470696494148183</v>
       </c>
       <c r="T15">
-        <v>-1.920497446251278</v>
+        <v>-0</v>
       </c>
       <c r="U15">
-        <v>1.920497446251278</v>
+        <v>1.470696494148183</v>
       </c>
       <c r="V15">
         <v>1.922</v>
       </c>
       <c r="W15">
-        <v>7.7811</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:23">
@@ -1603,28 +1603,28 @@
         <v>94.2</v>
       </c>
       <c r="C16">
-        <v>89.92825614072875</v>
+        <v>28.73258773467447</v>
       </c>
       <c r="D16">
-        <v>0.01434877185425121</v>
+        <v>-0.08982950347167562</v>
       </c>
       <c r="E16">
         <v>0.125</v>
       </c>
       <c r="F16">
-        <v>0.0007174385927125604</v>
+        <v>0.004491475173583781</v>
       </c>
       <c r="G16">
-        <v>0.7509851717917728</v>
+        <v>0.1918553320931964</v>
       </c>
       <c r="H16">
-        <v>0</v>
+        <v>0.008461939227031843</v>
       </c>
       <c r="I16">
-        <v>-0.5599975499052988</v>
+        <v>0</v>
       </c>
       <c r="J16">
-        <v>0.1592242757860308</v>
+        <v>0.1560600136942353</v>
       </c>
       <c r="K16" t="s">
         <v>49</v>
@@ -1639,31 +1639,31 @@
         <v>0</v>
       </c>
       <c r="O16">
-        <v>0.01434877185425121</v>
+        <v>0</v>
       </c>
       <c r="P16">
         <v>0</v>
       </c>
       <c r="Q16">
-        <v>-5.944772291988309</v>
+        <v>0</v>
       </c>
       <c r="R16">
-        <v>0</v>
+        <v>0.08982950347167562</v>
       </c>
       <c r="S16">
-        <v>-0</v>
+        <v>-1.656688043463219</v>
       </c>
       <c r="T16">
-        <v>-1.69027893615744</v>
+        <v>-0</v>
       </c>
       <c r="U16">
-        <v>1.69027893615744</v>
+        <v>1.656688043463219</v>
       </c>
       <c r="V16">
         <v>1.691</v>
       </c>
       <c r="W16">
-        <v>7.649400000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:23">
@@ -1674,28 +1674,28 @@
         <v>95</v>
       </c>
       <c r="C17">
-        <v>90</v>
+        <v>20</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>9.570888597260158</v>
       </c>
       <c r="E17">
         <v>0.125</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <v>0.4785444298630079</v>
       </c>
       <c r="G17">
-        <v>0.7036673816309533</v>
+        <v>-1.316801300087658</v>
       </c>
       <c r="H17">
         <v>0</v>
       </c>
       <c r="I17">
-        <v>-0.4790832988350333</v>
+        <v>0</v>
       </c>
       <c r="J17">
-        <v>0.1876267011649667</v>
+        <v>0</v>
       </c>
       <c r="K17" t="s">
         <v>49</v>
@@ -1713,10 +1713,10 @@
         <v>0</v>
       </c>
       <c r="P17">
-        <v>0</v>
+        <v>9.570888597260158</v>
       </c>
       <c r="Q17">
-        <v>-5.042982093000351</v>
+        <v>0</v>
       </c>
       <c r="R17">
         <v>0</v>
@@ -1725,16 +1725,16 @@
         <v>-0</v>
       </c>
       <c r="T17">
-        <v>-1.975017906999649</v>
+        <v>-0</v>
       </c>
       <c r="U17">
-        <v>1.975017906999649</v>
+        <v>0</v>
       </c>
       <c r="V17">
         <v>1.98</v>
       </c>
       <c r="W17">
-        <v>7.018</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:23">
@@ -1745,7 +1745,7 @@
         <v>98.7</v>
       </c>
       <c r="C18">
-        <v>90</v>
+        <v>67.8544429863008</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -1757,16 +1757,16 @@
         <v>0</v>
       </c>
       <c r="G18">
-        <v>0.6133189994537185</v>
+        <v>-0.008694395993434634</v>
       </c>
       <c r="H18">
         <v>0</v>
       </c>
       <c r="I18">
-        <v>-0.3909442403902012</v>
+        <v>0</v>
       </c>
       <c r="J18">
-        <v>0.1874081496097989</v>
+        <v>0.09112933500273557</v>
       </c>
       <c r="K18" t="s">
         <v>49</v>
@@ -1787,25 +1787,25 @@
         <v>0</v>
       </c>
       <c r="Q18">
-        <v>-3.960934553092211</v>
+        <v>0</v>
       </c>
       <c r="R18">
         <v>0</v>
       </c>
       <c r="S18">
-        <v>-0</v>
+        <v>-0.9232962006356187</v>
       </c>
       <c r="T18">
-        <v>-1.89876544690779</v>
+        <v>-0</v>
       </c>
       <c r="U18">
-        <v>1.89876544690779</v>
+        <v>0.9232962006356187</v>
       </c>
       <c r="V18">
         <v>1.92</v>
       </c>
       <c r="W18">
-        <v>5.859700000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:23">
@@ -1816,7 +1816,7 @@
         <v>102.5</v>
       </c>
       <c r="C19">
-        <v>90</v>
+        <v>63.23796198312269</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -1828,16 +1828,16 @@
         <v>0</v>
       </c>
       <c r="G19">
-        <v>0.4709918912341285</v>
+        <v>-0.1562102987179688</v>
       </c>
       <c r="H19">
         <v>0</v>
       </c>
       <c r="I19">
-        <v>-0.2632197919756225</v>
+        <v>0</v>
       </c>
       <c r="J19">
-        <v>0.1745167080243775</v>
+        <v>0.02285737553417968</v>
       </c>
       <c r="K19" t="s">
         <v>49</v>
@@ -1858,25 +1858,25 @@
         <v>0</v>
       </c>
       <c r="Q19">
-        <v>-2.567997970493878</v>
+        <v>0</v>
       </c>
       <c r="R19">
         <v>0</v>
       </c>
       <c r="S19">
-        <v>-0</v>
+        <v>-0.2229987856993139</v>
       </c>
       <c r="T19">
-        <v>-1.702602029506122</v>
+        <v>-0</v>
       </c>
       <c r="U19">
-        <v>1.702602029506122</v>
+        <v>0.2229987856993139</v>
       </c>
       <c r="V19">
         <v>1.716</v>
       </c>
       <c r="W19">
-        <v>4.2706</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:23">
@@ -1887,7 +1887,7 @@
         <v>107.86</v>
       </c>
       <c r="C20">
-        <v>90</v>
+        <v>62.12296805462613</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -1899,16 +1899,16 @@
         <v>0</v>
       </c>
       <c r="G20">
-        <v>0.2974855427783252</v>
+        <v>0.2366472498453367</v>
       </c>
       <c r="H20">
         <v>0</v>
       </c>
       <c r="I20">
-        <v>-0.04043894487262485</v>
+        <v>0</v>
       </c>
       <c r="J20">
-        <v>0.2146930991273752</v>
+        <v>0.2061933707688903</v>
       </c>
       <c r="K20" t="s">
         <v>49</v>
@@ -1929,25 +1929,25 @@
         <v>0</v>
       </c>
       <c r="Q20">
-        <v>-0.3749206830393552</v>
+        <v>0</v>
       </c>
       <c r="R20">
         <v>0</v>
       </c>
       <c r="S20">
-        <v>-0</v>
+        <v>-1.911675975977103</v>
       </c>
       <c r="T20">
-        <v>-1.990479316960645</v>
+        <v>-0</v>
       </c>
       <c r="U20">
-        <v>1.990479316960645</v>
+        <v>1.911675975977103</v>
       </c>
       <c r="V20">
         <v>1.995</v>
       </c>
       <c r="W20">
-        <v>2.3654</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:23">
@@ -1958,7 +1958,7 @@
         <v>151</v>
       </c>
       <c r="C21">
-        <v>90</v>
+        <v>52.56458817474061</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -1970,7 +1970,7 @@
         <v>0</v>
       </c>
       <c r="G21">
-        <v>0.2865811706973438</v>
+        <v>0.280974756468153</v>
       </c>
       <c r="H21">
         <v>0</v>
@@ -1979,7 +1979,7 @@
         <v>0</v>
       </c>
       <c r="J21">
-        <v>0.2391518211238932</v>
+        <v>0.2368158151950638</v>
       </c>
       <c r="K21" t="s">
         <v>49</v>
@@ -2006,19 +2006,19 @@
         <v>0</v>
       </c>
       <c r="S21">
-        <v>-1.04478689486022</v>
+        <v>-1.568316656920952</v>
       </c>
       <c r="T21">
-        <v>-0.539</v>
+        <v>-0</v>
       </c>
       <c r="U21">
-        <v>1.58378689486022</v>
+        <v>1.568316656920952</v>
       </c>
       <c r="V21">
         <v>1.586</v>
       </c>
       <c r="W21">
-        <v>0.539</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:23">
@@ -2029,28 +2029,28 @@
         <v>149.85</v>
       </c>
       <c r="C22">
-        <v>84.7760655256989</v>
+        <v>44.72300489013585</v>
       </c>
       <c r="D22">
-        <v>-3.973845061920404</v>
+        <v>0</v>
       </c>
       <c r="E22">
         <v>0.125</v>
       </c>
       <c r="F22">
-        <v>0.1986922530960202</v>
+        <v>0</v>
       </c>
       <c r="G22">
-        <v>0.9568295182350837</v>
+        <v>0.3500536064002543</v>
       </c>
       <c r="H22">
-        <v>0.5954806825287726</v>
+        <v>0</v>
       </c>
       <c r="I22">
         <v>0</v>
       </c>
       <c r="J22">
-        <v>0.3034839398776296</v>
+        <v>0.2987775943334393</v>
       </c>
       <c r="K22" t="s">
         <v>49</v>
@@ -2074,22 +2074,22 @@
         <v>0</v>
       </c>
       <c r="R22">
-        <v>3.973845061920404</v>
+        <v>0</v>
       </c>
       <c r="S22">
-        <v>-1.888051517368232</v>
+        <v>-1.993844473362958</v>
       </c>
       <c r="T22">
-        <v>-0.1372</v>
+        <v>-0</v>
       </c>
       <c r="U22">
-        <v>2.025251517368232</v>
+        <v>1.993844473362958</v>
       </c>
       <c r="V22">
         <v>2.041</v>
       </c>
       <c r="W22">
-        <v>0.1372</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:23">
@@ -2100,7 +2100,7 @@
         <v>133.8</v>
       </c>
       <c r="C23">
-        <v>55.46658262925571</v>
+        <v>34.75378252332106</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -2112,7 +2112,7 @@
         <v>0</v>
       </c>
       <c r="G23">
-        <v>0.3132436138822211</v>
+        <v>0.267690361013885</v>
       </c>
       <c r="H23">
         <v>0</v>
@@ -2121,7 +2121,7 @@
         <v>0</v>
       </c>
       <c r="J23">
-        <v>0.2619097724509254</v>
+        <v>0.2429292504224521</v>
       </c>
       <c r="K23" t="s">
         <v>49</v>
@@ -2148,13 +2148,13 @@
         <v>0</v>
       </c>
       <c r="S23">
-        <v>-1.95747214088883</v>
+        <v>-1.815614726625202</v>
       </c>
       <c r="T23">
         <v>-0</v>
       </c>
       <c r="U23">
-        <v>1.95747214088883</v>
+        <v>1.815614726625202</v>
       </c>
       <c r="V23">
         <v>1.964</v>
@@ -2171,7 +2171,7 @@
         <v>103.85</v>
       </c>
       <c r="C24">
-        <v>45.67922192481156</v>
+        <v>25.67570889019505</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -2183,7 +2183,7 @@
         <v>0</v>
       </c>
       <c r="G24">
-        <v>0.2261639410261073</v>
+        <v>-0.01069033521125611</v>
       </c>
       <c r="H24">
         <v>0</v>
@@ -2192,7 +2192,7 @@
         <v>0</v>
       </c>
       <c r="J24">
-        <v>0.1906077754275447</v>
+        <v>0.09191849366197663</v>
       </c>
       <c r="K24" t="s">
         <v>49</v>
@@ -2219,13 +2219,13 @@
         <v>0</v>
       </c>
       <c r="S24">
-        <v>-1.835414303587335</v>
+        <v>-0.885108268290579</v>
       </c>
       <c r="T24">
         <v>-0</v>
       </c>
       <c r="U24">
-        <v>1.835414303587335</v>
+        <v>0.885108268290579</v>
       </c>
       <c r="V24">
         <v>1.856</v>
@@ -2242,7 +2242,7 @@
         <v>96</v>
       </c>
       <c r="C25">
-        <v>36.50215040687489</v>
+        <v>21.25016754874216</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -2254,7 +2254,7 @@
         <v>0</v>
       </c>
       <c r="G25">
-        <v>0.1831422753691164</v>
+        <v>-0.1454136968490627</v>
       </c>
       <c r="H25">
         <v>0</v>
@@ -2263,7 +2263,7 @@
         <v>0</v>
       </c>
       <c r="J25">
-        <v>0.1573332814037985</v>
+        <v>0.02043495964622389</v>
       </c>
       <c r="K25" t="s">
         <v>49</v>
@@ -2290,13 +2290,13 @@
         <v>0</v>
       </c>
       <c r="S25">
-        <v>-1.638888347956234</v>
+        <v>-0.2128641629814988</v>
       </c>
       <c r="T25">
         <v>-0</v>
       </c>
       <c r="U25">
-        <v>1.638888347956234</v>
+        <v>0.2128641629814988</v>
       </c>
       <c r="V25">
         <v>1.688</v>
@@ -2313,28 +2313,28 @@
         <v>102.95</v>
       </c>
       <c r="C26">
-        <v>28.30770866709372</v>
+        <v>20.18584673383467</v>
       </c>
       <c r="D26">
-        <v>-0.008479629924323051</v>
+        <v>0</v>
       </c>
       <c r="E26">
         <v>0.125</v>
       </c>
       <c r="F26">
-        <v>0.0004239814962161526</v>
+        <v>0</v>
       </c>
       <c r="G26">
-        <v>0.2042351624321104</v>
+        <v>-0.199987694159988</v>
       </c>
       <c r="H26">
-        <v>0.0008729779007090582</v>
+        <v>0</v>
       </c>
       <c r="I26">
         <v>0</v>
       </c>
       <c r="J26">
-        <v>0.1701827435547506</v>
+        <v>0.002120294100004973</v>
       </c>
       <c r="K26" t="s">
         <v>49</v>
@@ -2358,16 +2358,16 @@
         <v>0</v>
       </c>
       <c r="R26">
-        <v>0.008479629924323051</v>
+        <v>0</v>
       </c>
       <c r="S26">
-        <v>-1.65306210349442</v>
+        <v>-0.02059537736770251</v>
       </c>
       <c r="T26">
         <v>-0</v>
       </c>
       <c r="U26">
-        <v>1.65306210349442</v>
+        <v>0.02059537736770251</v>
       </c>
       <c r="V26">
         <v>1.66</v>
@@ -2384,7 +2384,7 @@
         <v>100.85</v>
       </c>
       <c r="C27">
-        <v>20</v>
+        <v>20.08286984699615</v>
       </c>
       <c r="D27">
         <v>0</v>

</xml_diff>

<commit_message>
Updating Load default parameters
</commit_message>
<xml_diff>
--- a/data/Output/xlsx/results.xlsx
+++ b/data/Output/xlsx/results.xlsx
@@ -612,25 +612,25 @@
         <v>60</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>-1.517586829436955</v>
       </c>
       <c r="E2">
         <v>0.125</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>0.07587934147184777</v>
       </c>
       <c r="G2">
-        <v>0.1294427768909185</v>
+        <v>0.1490118507824147</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>0.1490118507824147</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
       <c r="J2">
-        <v>0.136021330371216</v>
+        <v>0</v>
       </c>
       <c r="K2" t="s">
         <v>49</v>
@@ -654,19 +654,19 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>0</v>
+        <v>1.517586829436955</v>
       </c>
       <c r="S2">
-        <v>-1.385286998382891</v>
+        <v>-0</v>
       </c>
       <c r="T2">
         <v>-0</v>
       </c>
       <c r="U2">
-        <v>1.385286998382891</v>
+        <v>0</v>
       </c>
       <c r="V2">
-        <v>1.672</v>
+        <v>0</v>
       </c>
       <c r="W2">
         <v>0</v>
@@ -680,19 +680,19 @@
         <v>97.36</v>
       </c>
       <c r="C3">
-        <v>53.07356500808555</v>
+        <v>52.41206585281522</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>0.7891180289236067</v>
       </c>
       <c r="E3">
         <v>0.125</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>0.03945590144618034</v>
       </c>
       <c r="G3">
-        <v>0.1839686096833563</v>
+        <v>-0.07682853129600235</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -701,7 +701,7 @@
         <v>0</v>
       </c>
       <c r="J3">
-        <v>0.1678799073680652</v>
+        <v>0</v>
       </c>
       <c r="K3" t="s">
         <v>49</v>
@@ -719,7 +719,7 @@
         <v>0</v>
       </c>
       <c r="P3">
-        <v>0</v>
+        <v>0.7891180289236067</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -728,16 +728,16 @@
         <v>0</v>
       </c>
       <c r="S3">
-        <v>-1.724321152095986</v>
+        <v>-0</v>
       </c>
       <c r="T3">
         <v>-0</v>
       </c>
       <c r="U3">
-        <v>1.724321152095986</v>
+        <v>0</v>
       </c>
       <c r="V3">
-        <v>1.874</v>
+        <v>0</v>
       </c>
       <c r="W3">
         <v>0</v>
@@ -751,19 +751,19 @@
         <v>97.15000000000001</v>
       </c>
       <c r="C4">
-        <v>44.45195924760561</v>
+        <v>56.35765599743326</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>5.473934116369112</v>
       </c>
       <c r="E4">
         <v>0.125</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>0.2736967058184556</v>
       </c>
       <c r="G4">
-        <v>0.1960820334845552</v>
+        <v>-0.5317926994052593</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -772,7 +772,7 @@
         <v>0</v>
       </c>
       <c r="J4">
-        <v>0.1637440222852313</v>
+        <v>0</v>
       </c>
       <c r="K4" t="s">
         <v>49</v>
@@ -790,7 +790,7 @@
         <v>0</v>
       </c>
       <c r="P4">
-        <v>0</v>
+        <v>5.473934116369112</v>
       </c>
       <c r="Q4">
         <v>0</v>
@@ -799,16 +799,16 @@
         <v>0</v>
       </c>
       <c r="S4">
-        <v>-1.685476297326107</v>
+        <v>-0</v>
       </c>
       <c r="T4">
         <v>-0</v>
       </c>
       <c r="U4">
-        <v>1.685476297326107</v>
+        <v>0</v>
       </c>
       <c r="V4">
-        <v>1.689</v>
+        <v>0</v>
       </c>
       <c r="W4">
         <v>0</v>
@@ -822,19 +822,19 @@
         <v>96.66</v>
       </c>
       <c r="C5">
-        <v>36.02457776097508</v>
+        <v>83.72732657927881</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>1.254534684144237</v>
       </c>
       <c r="E5">
         <v>0.125</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>0.06272673420721186</v>
       </c>
       <c r="G5">
-        <v>0.1425237157371368</v>
+        <v>-0.121263322569382</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -843,7 +843,7 @@
         <v>0</v>
       </c>
       <c r="J5">
-        <v>0.1389360615571403</v>
+        <v>0</v>
       </c>
       <c r="K5" t="s">
         <v>49</v>
@@ -861,7 +861,7 @@
         <v>0</v>
       </c>
       <c r="P5">
-        <v>0</v>
+        <v>1.254534684144237</v>
       </c>
       <c r="Q5">
         <v>0</v>
@@ -870,16 +870,16 @@
         <v>0</v>
       </c>
       <c r="S5">
-        <v>-1.437368731193258</v>
+        <v>-0</v>
       </c>
       <c r="T5">
         <v>-0</v>
       </c>
       <c r="U5">
-        <v>1.437368731193258</v>
+        <v>0</v>
       </c>
       <c r="V5">
-        <v>1.646</v>
+        <v>0</v>
       </c>
       <c r="W5">
         <v>0</v>
@@ -893,28 +893,28 @@
         <v>97.98</v>
       </c>
       <c r="C6">
-        <v>28.83773410500879</v>
+        <v>90</v>
       </c>
       <c r="D6">
-        <v>-0.02066547782790784</v>
+        <v>0</v>
       </c>
       <c r="E6">
         <v>0.125</v>
       </c>
       <c r="F6">
-        <v>0.001033273891395392</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <v>0.1854154611275955</v>
+        <v>0</v>
       </c>
       <c r="H6">
-        <v>0.00202480351757841</v>
+        <v>0</v>
       </c>
       <c r="I6">
         <v>0</v>
       </c>
       <c r="J6">
-        <v>0.1711594340041738</v>
+        <v>0</v>
       </c>
       <c r="K6" t="s">
         <v>49</v>
@@ -938,19 +938,19 @@
         <v>0</v>
       </c>
       <c r="R6">
-        <v>0.02066547782790784</v>
+        <v>0</v>
       </c>
       <c r="S6">
-        <v>-1.74688134317385</v>
+        <v>-0</v>
       </c>
       <c r="T6">
         <v>-0</v>
       </c>
       <c r="U6">
-        <v>1.74688134317385</v>
+        <v>0</v>
       </c>
       <c r="V6">
-        <v>1.934</v>
+        <v>0</v>
       </c>
       <c r="W6">
         <v>0</v>
@@ -964,19 +964,19 @@
         <v>89.55</v>
       </c>
       <c r="C7">
-        <v>20</v>
+        <v>90</v>
       </c>
       <c r="D7">
-        <v>9.570888597260158</v>
+        <v>0</v>
       </c>
       <c r="E7">
         <v>0.125</v>
       </c>
       <c r="F7">
-        <v>0.4785444298630079</v>
+        <v>0</v>
       </c>
       <c r="G7">
-        <v>-1.214500948661576</v>
+        <v>0</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -1003,7 +1003,7 @@
         <v>0</v>
       </c>
       <c r="P7">
-        <v>9.570888597260158</v>
+        <v>0</v>
       </c>
       <c r="Q7">
         <v>0</v>
@@ -1021,7 +1021,7 @@
         <v>0</v>
       </c>
       <c r="V7">
-        <v>1.731</v>
+        <v>0</v>
       </c>
       <c r="W7">
         <v>0</v>
@@ -1035,7 +1035,7 @@
         <v>104.21</v>
       </c>
       <c r="C8">
-        <v>67.8544429863008</v>
+        <v>90</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1047,7 +1047,7 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <v>0.09576465376964684</v>
+        <v>0</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -1056,7 +1056,7 @@
         <v>0</v>
       </c>
       <c r="J8">
-        <v>0.1544808340706862</v>
+        <v>0</v>
       </c>
       <c r="K8" t="s">
         <v>49</v>
@@ -1083,16 +1083,16 @@
         <v>0</v>
       </c>
       <c r="S8">
-        <v>-1.482399328957741</v>
+        <v>-0</v>
       </c>
       <c r="T8">
         <v>-0</v>
       </c>
       <c r="U8">
-        <v>1.482399328957741</v>
+        <v>0</v>
       </c>
       <c r="V8">
-        <v>2.199</v>
+        <v>0</v>
       </c>
       <c r="W8">
         <v>0</v>
@@ -1106,28 +1106,28 @@
         <v>118.21</v>
       </c>
       <c r="C9">
-        <v>60.44244634151208</v>
+        <v>90</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>-4.195753223810646</v>
       </c>
       <c r="E9">
         <v>0.125</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>0.2097876611905323</v>
       </c>
       <c r="G9">
-        <v>0.1840019904277628</v>
+        <v>0.4959799885866565</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>0.4959799885866565</v>
       </c>
       <c r="I9">
         <v>0</v>
       </c>
       <c r="J9">
-        <v>0.1728313310115678</v>
+        <v>0</v>
       </c>
       <c r="K9" t="s">
         <v>49</v>
@@ -1151,19 +1151,19 @@
         <v>0</v>
       </c>
       <c r="R9">
-        <v>0</v>
+        <v>4.195753223810646</v>
       </c>
       <c r="S9">
-        <v>-1.462070307178478</v>
+        <v>-0</v>
       </c>
       <c r="T9">
         <v>-0</v>
       </c>
       <c r="U9">
-        <v>1.462070307178478</v>
+        <v>0</v>
       </c>
       <c r="V9">
-        <v>1.627</v>
+        <v>0</v>
       </c>
       <c r="W9">
         <v>0</v>
@@ -1177,28 +1177,28 @@
         <v>145</v>
       </c>
       <c r="C10">
-        <v>53.13209480561969</v>
+        <v>69.02123388094677</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>-4.015976791473788</v>
       </c>
       <c r="E10">
         <v>0.125</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>0.2007988395736894</v>
       </c>
       <c r="G10">
-        <v>0.2625408050941181</v>
+        <v>0.5823166347636993</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>0.5823166347636993</v>
       </c>
       <c r="I10">
         <v>0</v>
       </c>
       <c r="J10">
-        <v>0.2350345021225493</v>
+        <v>0</v>
       </c>
       <c r="K10" t="s">
         <v>49</v>
@@ -1222,19 +1222,19 @@
         <v>0</v>
       </c>
       <c r="R10">
-        <v>0</v>
+        <v>4.015976791473788</v>
       </c>
       <c r="S10">
-        <v>-1.620927600845167</v>
+        <v>-0</v>
       </c>
       <c r="T10">
         <v>-0</v>
       </c>
       <c r="U10">
-        <v>1.620927600845167</v>
+        <v>0</v>
       </c>
       <c r="V10">
-        <v>1.733</v>
+        <v>0</v>
       </c>
       <c r="W10">
         <v>0</v>
@@ -1248,28 +1248,28 @@
         <v>129.42</v>
       </c>
       <c r="C11">
-        <v>45.02745680139385</v>
+        <v>48.94134992357782</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>-3.826771154896456</v>
       </c>
       <c r="E11">
         <v>0.125</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>0.1913385577448228</v>
       </c>
       <c r="G11">
-        <v>0.2899672715031826</v>
+        <v>0.4952607228666992</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>0.4952607228666992</v>
       </c>
       <c r="I11">
         <v>0</v>
       </c>
       <c r="J11">
-        <v>0.2513397664596594</v>
+        <v>0</v>
       </c>
       <c r="K11" t="s">
         <v>49</v>
@@ -1293,19 +1293,19 @@
         <v>0</v>
       </c>
       <c r="R11">
-        <v>0</v>
+        <v>3.826771154896456</v>
       </c>
       <c r="S11">
-        <v>-1.942047337812235</v>
+        <v>-0</v>
       </c>
       <c r="T11">
         <v>-0</v>
       </c>
       <c r="U11">
-        <v>1.942047337812235</v>
+        <v>0</v>
       </c>
       <c r="V11">
-        <v>2.017</v>
+        <v>0</v>
       </c>
       <c r="W11">
         <v>0</v>
@@ -1319,28 +1319,28 @@
         <v>100.82</v>
       </c>
       <c r="C12">
-        <v>35.31722011233268</v>
+        <v>29.80749414909555</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>-1.961498829819109</v>
       </c>
       <c r="E12">
         <v>0.125</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>0.09807494149095547</v>
       </c>
       <c r="G12">
-        <v>0.226580851315367</v>
+        <v>0.1977583120223626</v>
       </c>
       <c r="H12">
-        <v>0</v>
+        <v>0.1977583120223626</v>
       </c>
       <c r="I12">
         <v>0</v>
       </c>
       <c r="J12">
-        <v>0.1902380980480696</v>
+        <v>0</v>
       </c>
       <c r="K12" t="s">
         <v>49</v>
@@ -1364,19 +1364,19 @@
         <v>0</v>
       </c>
       <c r="R12">
-        <v>0</v>
+        <v>1.961498829819109</v>
       </c>
       <c r="S12">
-        <v>-1.886908332157008</v>
+        <v>-0</v>
       </c>
       <c r="T12">
         <v>-0</v>
       </c>
       <c r="U12">
-        <v>1.886908332157008</v>
+        <v>0</v>
       </c>
       <c r="V12">
-        <v>1.901</v>
+        <v>0</v>
       </c>
       <c r="W12">
         <v>0</v>
@@ -1390,28 +1390,28 @@
         <v>94.12</v>
       </c>
       <c r="C13">
-        <v>25.88267845154764</v>
+        <v>20</v>
       </c>
       <c r="D13">
-        <v>-0.04914236872111433</v>
+        <v>0.01468583641022033</v>
       </c>
       <c r="E13">
         <v>0.125</v>
       </c>
       <c r="F13">
-        <v>0.002457118436055716</v>
+        <v>0.0007342918205110166</v>
       </c>
       <c r="G13">
-        <v>0.04379275037099467</v>
+        <v>-0.001382230922929938</v>
       </c>
       <c r="H13">
-        <v>0.004625279744031281</v>
+        <v>0</v>
       </c>
       <c r="I13">
         <v>0</v>
       </c>
       <c r="J13">
-        <v>0.1061102594279014</v>
+        <v>0</v>
       </c>
       <c r="K13" t="s">
         <v>49</v>
@@ -1429,25 +1429,25 @@
         <v>0</v>
       </c>
       <c r="P13">
-        <v>0</v>
+        <v>0.01468583641022033</v>
       </c>
       <c r="Q13">
         <v>0</v>
       </c>
       <c r="R13">
-        <v>0.04914236872111433</v>
+        <v>0</v>
       </c>
       <c r="S13">
-        <v>-1.127393321588413</v>
+        <v>-0</v>
       </c>
       <c r="T13">
         <v>-0</v>
       </c>
       <c r="U13">
-        <v>1.127393321588413</v>
+        <v>0</v>
       </c>
       <c r="V13">
-        <v>1.908</v>
+        <v>0</v>
       </c>
       <c r="W13">
         <v>0</v>
@@ -1461,19 +1461,19 @@
         <v>82.59999999999999</v>
       </c>
       <c r="C14">
-        <v>20</v>
+        <v>20.0734291820511</v>
       </c>
       <c r="D14">
-        <v>3.217214041083077</v>
+        <v>9.570397286250321</v>
       </c>
       <c r="E14">
         <v>0.125</v>
       </c>
       <c r="F14">
-        <v>0.1608607020541538</v>
+        <v>0.478519864312516</v>
       </c>
       <c r="G14">
-        <v>-0.4900704957521546</v>
+        <v>-0.7905148158442764</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -1500,7 +1500,7 @@
         <v>0</v>
       </c>
       <c r="P14">
-        <v>3.217214041083077</v>
+        <v>9.570397286250321</v>
       </c>
       <c r="Q14">
         <v>0</v>
@@ -1518,7 +1518,7 @@
         <v>0</v>
       </c>
       <c r="V14">
-        <v>1.727</v>
+        <v>0</v>
       </c>
       <c r="W14">
         <v>0</v>
@@ -1532,19 +1532,19 @@
         <v>85.59999999999999</v>
       </c>
       <c r="C15">
-        <v>36.08607020541539</v>
+        <v>67.9254156133027</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>4.414916877339459</v>
       </c>
       <c r="E15">
         <v>0.125</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>0.2207458438669729</v>
       </c>
       <c r="G15">
-        <v>0.1047120477578028</v>
+        <v>-0.3779168847002576</v>
       </c>
       <c r="H15">
         <v>0</v>
@@ -1553,7 +1553,7 @@
         <v>0</v>
       </c>
       <c r="J15">
-        <v>0.1258916198990845</v>
+        <v>0</v>
       </c>
       <c r="K15" t="s">
         <v>49</v>
@@ -1571,7 +1571,7 @@
         <v>0</v>
       </c>
       <c r="P15">
-        <v>0</v>
+        <v>4.414916877339459</v>
       </c>
       <c r="Q15">
         <v>0</v>
@@ -1580,16 +1580,16 @@
         <v>0</v>
       </c>
       <c r="S15">
-        <v>-1.470696494148183</v>
+        <v>-0</v>
       </c>
       <c r="T15">
         <v>-0</v>
       </c>
       <c r="U15">
-        <v>1.470696494148183</v>
+        <v>0</v>
       </c>
       <c r="V15">
-        <v>1.922</v>
+        <v>0</v>
       </c>
       <c r="W15">
         <v>0</v>
@@ -1603,28 +1603,28 @@
         <v>94.2</v>
       </c>
       <c r="C16">
-        <v>28.73258773467447</v>
+        <v>90</v>
       </c>
       <c r="D16">
-        <v>-0.08982950347167562</v>
+        <v>0</v>
       </c>
       <c r="E16">
         <v>0.125</v>
       </c>
       <c r="F16">
-        <v>0.004491475173583781</v>
+        <v>0</v>
       </c>
       <c r="G16">
-        <v>0.1918553320931964</v>
+        <v>0</v>
       </c>
       <c r="H16">
-        <v>0.008461939227031843</v>
+        <v>0</v>
       </c>
       <c r="I16">
         <v>0</v>
       </c>
       <c r="J16">
-        <v>0.1560600136942353</v>
+        <v>0</v>
       </c>
       <c r="K16" t="s">
         <v>49</v>
@@ -1648,19 +1648,19 @@
         <v>0</v>
       </c>
       <c r="R16">
-        <v>0.08982950347167562</v>
+        <v>0</v>
       </c>
       <c r="S16">
-        <v>-1.656688043463219</v>
+        <v>-0</v>
       </c>
       <c r="T16">
         <v>-0</v>
       </c>
       <c r="U16">
-        <v>1.656688043463219</v>
+        <v>0</v>
       </c>
       <c r="V16">
-        <v>1.691</v>
+        <v>0</v>
       </c>
       <c r="W16">
         <v>0</v>
@@ -1674,19 +1674,19 @@
         <v>95</v>
       </c>
       <c r="C17">
-        <v>20</v>
+        <v>90</v>
       </c>
       <c r="D17">
-        <v>9.570888597260158</v>
+        <v>0</v>
       </c>
       <c r="E17">
         <v>0.125</v>
       </c>
       <c r="F17">
-        <v>0.4785444298630079</v>
+        <v>0</v>
       </c>
       <c r="G17">
-        <v>-1.316801300087658</v>
+        <v>0</v>
       </c>
       <c r="H17">
         <v>0</v>
@@ -1713,7 +1713,7 @@
         <v>0</v>
       </c>
       <c r="P17">
-        <v>9.570888597260158</v>
+        <v>0</v>
       </c>
       <c r="Q17">
         <v>0</v>
@@ -1731,7 +1731,7 @@
         <v>0</v>
       </c>
       <c r="V17">
-        <v>1.98</v>
+        <v>0</v>
       </c>
       <c r="W17">
         <v>0</v>
@@ -1745,7 +1745,7 @@
         <v>98.7</v>
       </c>
       <c r="C18">
-        <v>67.8544429863008</v>
+        <v>90</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -1757,7 +1757,7 @@
         <v>0</v>
       </c>
       <c r="G18">
-        <v>-0.008694395993434634</v>
+        <v>0</v>
       </c>
       <c r="H18">
         <v>0</v>
@@ -1766,7 +1766,7 @@
         <v>0</v>
       </c>
       <c r="J18">
-        <v>0.09112933500273557</v>
+        <v>0</v>
       </c>
       <c r="K18" t="s">
         <v>49</v>
@@ -1793,16 +1793,16 @@
         <v>0</v>
       </c>
       <c r="S18">
-        <v>-0.9232962006356187</v>
+        <v>-0</v>
       </c>
       <c r="T18">
         <v>-0</v>
       </c>
       <c r="U18">
-        <v>0.9232962006356187</v>
+        <v>0</v>
       </c>
       <c r="V18">
-        <v>1.92</v>
+        <v>0</v>
       </c>
       <c r="W18">
         <v>0</v>
@@ -1816,7 +1816,7 @@
         <v>102.5</v>
       </c>
       <c r="C19">
-        <v>63.23796198312269</v>
+        <v>90</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -1828,7 +1828,7 @@
         <v>0</v>
       </c>
       <c r="G19">
-        <v>-0.1562102987179688</v>
+        <v>0</v>
       </c>
       <c r="H19">
         <v>0</v>
@@ -1837,7 +1837,7 @@
         <v>0</v>
       </c>
       <c r="J19">
-        <v>0.02285737553417968</v>
+        <v>0</v>
       </c>
       <c r="K19" t="s">
         <v>49</v>
@@ -1864,16 +1864,16 @@
         <v>0</v>
       </c>
       <c r="S19">
-        <v>-0.2229987856993139</v>
+        <v>-0</v>
       </c>
       <c r="T19">
         <v>-0</v>
       </c>
       <c r="U19">
-        <v>0.2229987856993139</v>
+        <v>0</v>
       </c>
       <c r="V19">
-        <v>1.716</v>
+        <v>0</v>
       </c>
       <c r="W19">
         <v>0</v>
@@ -1887,7 +1887,7 @@
         <v>107.86</v>
       </c>
       <c r="C20">
-        <v>62.12296805462613</v>
+        <v>90</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -1899,7 +1899,7 @@
         <v>0</v>
       </c>
       <c r="G20">
-        <v>0.2366472498453367</v>
+        <v>0</v>
       </c>
       <c r="H20">
         <v>0</v>
@@ -1908,7 +1908,7 @@
         <v>0</v>
       </c>
       <c r="J20">
-        <v>0.2061933707688903</v>
+        <v>0</v>
       </c>
       <c r="K20" t="s">
         <v>49</v>
@@ -1935,16 +1935,16 @@
         <v>0</v>
       </c>
       <c r="S20">
-        <v>-1.911675975977103</v>
+        <v>-0</v>
       </c>
       <c r="T20">
         <v>-0</v>
       </c>
       <c r="U20">
-        <v>1.911675975977103</v>
+        <v>0</v>
       </c>
       <c r="V20">
-        <v>1.995</v>
+        <v>0</v>
       </c>
       <c r="W20">
         <v>0</v>
@@ -1958,28 +1958,28 @@
         <v>151</v>
       </c>
       <c r="C21">
-        <v>52.56458817474061</v>
+        <v>90</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>-4.195753223810646</v>
       </c>
       <c r="E21">
         <v>0.125</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>0.2097876611905323</v>
       </c>
       <c r="G21">
-        <v>0.280974756468153</v>
+        <v>0.6335587367954076</v>
       </c>
       <c r="H21">
-        <v>0</v>
+        <v>0.6335587367954076</v>
       </c>
       <c r="I21">
         <v>0</v>
       </c>
       <c r="J21">
-        <v>0.2368158151950638</v>
+        <v>0</v>
       </c>
       <c r="K21" t="s">
         <v>49</v>
@@ -2003,19 +2003,19 @@
         <v>0</v>
       </c>
       <c r="R21">
-        <v>0</v>
+        <v>4.195753223810646</v>
       </c>
       <c r="S21">
-        <v>-1.568316656920952</v>
+        <v>-0</v>
       </c>
       <c r="T21">
         <v>-0</v>
       </c>
       <c r="U21">
-        <v>1.568316656920952</v>
+        <v>0</v>
       </c>
       <c r="V21">
-        <v>1.586</v>
+        <v>0</v>
       </c>
       <c r="W21">
         <v>0</v>
@@ -2029,28 +2029,28 @@
         <v>149.85</v>
       </c>
       <c r="C22">
-        <v>44.72300489013585</v>
+        <v>69.02123388094677</v>
       </c>
       <c r="D22">
-        <v>0</v>
+        <v>-4.015976791473788</v>
       </c>
       <c r="E22">
         <v>0.125</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>0.2007988395736894</v>
       </c>
       <c r="G22">
-        <v>0.3500536064002543</v>
+        <v>0.6017941222023471</v>
       </c>
       <c r="H22">
-        <v>0</v>
+        <v>0.6017941222023471</v>
       </c>
       <c r="I22">
         <v>0</v>
       </c>
       <c r="J22">
-        <v>0.2987775943334393</v>
+        <v>0</v>
       </c>
       <c r="K22" t="s">
         <v>49</v>
@@ -2074,19 +2074,19 @@
         <v>0</v>
       </c>
       <c r="R22">
-        <v>0</v>
+        <v>4.015976791473788</v>
       </c>
       <c r="S22">
-        <v>-1.993844473362958</v>
+        <v>-0</v>
       </c>
       <c r="T22">
         <v>-0</v>
       </c>
       <c r="U22">
-        <v>1.993844473362958</v>
+        <v>0</v>
       </c>
       <c r="V22">
-        <v>2.041</v>
+        <v>0</v>
       </c>
       <c r="W22">
         <v>0</v>
@@ -2100,28 +2100,28 @@
         <v>133.8</v>
       </c>
       <c r="C23">
-        <v>34.75378252332106</v>
+        <v>48.94134992357782</v>
       </c>
       <c r="D23">
-        <v>0</v>
+        <v>-3.826771154896456</v>
       </c>
       <c r="E23">
         <v>0.125</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>0.1913385577448228</v>
       </c>
       <c r="G23">
-        <v>0.267690361013885</v>
+        <v>0.5120219805251458</v>
       </c>
       <c r="H23">
-        <v>0</v>
+        <v>0.5120219805251458</v>
       </c>
       <c r="I23">
         <v>0</v>
       </c>
       <c r="J23">
-        <v>0.2429292504224521</v>
+        <v>0</v>
       </c>
       <c r="K23" t="s">
         <v>49</v>
@@ -2145,19 +2145,19 @@
         <v>0</v>
       </c>
       <c r="R23">
-        <v>0</v>
+        <v>3.826771154896456</v>
       </c>
       <c r="S23">
-        <v>-1.815614726625202</v>
+        <v>-0</v>
       </c>
       <c r="T23">
         <v>-0</v>
       </c>
       <c r="U23">
-        <v>1.815614726625202</v>
+        <v>0</v>
       </c>
       <c r="V23">
-        <v>1.964</v>
+        <v>0</v>
       </c>
       <c r="W23">
         <v>0</v>
@@ -2171,28 +2171,28 @@
         <v>103.85</v>
       </c>
       <c r="C24">
-        <v>25.67570889019505</v>
+        <v>29.80749414909555</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>-1.961498829819109</v>
       </c>
       <c r="E24">
         <v>0.125</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>0.09807494149095547</v>
       </c>
       <c r="G24">
-        <v>-0.01069033521125611</v>
+        <v>0.2037016534767145</v>
       </c>
       <c r="H24">
-        <v>0</v>
+        <v>0.2037016534767145</v>
       </c>
       <c r="I24">
         <v>0</v>
       </c>
       <c r="J24">
-        <v>0.09191849366197663</v>
+        <v>0</v>
       </c>
       <c r="K24" t="s">
         <v>49</v>
@@ -2216,19 +2216,19 @@
         <v>0</v>
       </c>
       <c r="R24">
-        <v>0</v>
+        <v>1.961498829819109</v>
       </c>
       <c r="S24">
-        <v>-0.885108268290579</v>
+        <v>-0</v>
       </c>
       <c r="T24">
         <v>-0</v>
       </c>
       <c r="U24">
-        <v>0.885108268290579</v>
+        <v>0</v>
       </c>
       <c r="V24">
-        <v>1.856</v>
+        <v>0</v>
       </c>
       <c r="W24">
         <v>0</v>
@@ -2242,19 +2242,19 @@
         <v>96</v>
       </c>
       <c r="C25">
-        <v>21.25016754874216</v>
+        <v>20</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <v>2.430912548402899</v>
       </c>
       <c r="E25">
         <v>0.125</v>
       </c>
       <c r="F25">
-        <v>0</v>
+        <v>0.1215456274201449</v>
       </c>
       <c r="G25">
-        <v>-0.1454136968490627</v>
+        <v>-0.2333676046466783</v>
       </c>
       <c r="H25">
         <v>0</v>
@@ -2263,7 +2263,7 @@
         <v>0</v>
       </c>
       <c r="J25">
-        <v>0.02043495964622389</v>
+        <v>0</v>
       </c>
       <c r="K25" t="s">
         <v>49</v>
@@ -2281,7 +2281,7 @@
         <v>0</v>
       </c>
       <c r="P25">
-        <v>0</v>
+        <v>2.430912548402899</v>
       </c>
       <c r="Q25">
         <v>0</v>
@@ -2290,16 +2290,16 @@
         <v>0</v>
       </c>
       <c r="S25">
-        <v>-0.2128641629814988</v>
+        <v>-0</v>
       </c>
       <c r="T25">
         <v>-0</v>
       </c>
       <c r="U25">
-        <v>0.2128641629814988</v>
+        <v>0</v>
       </c>
       <c r="V25">
-        <v>1.688</v>
+        <v>0</v>
       </c>
       <c r="W25">
         <v>0</v>
@@ -2313,28 +2313,28 @@
         <v>102.95</v>
       </c>
       <c r="C26">
-        <v>20.18584673383467</v>
+        <v>32.15456274201449</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>-2.430912548402898</v>
       </c>
       <c r="E26">
         <v>0.125</v>
       </c>
       <c r="F26">
-        <v>0</v>
+        <v>0.1215456274201449</v>
       </c>
       <c r="G26">
-        <v>-0.199987694159988</v>
+        <v>0.2502624468580784</v>
       </c>
       <c r="H26">
-        <v>0</v>
+        <v>0.2502624468580784</v>
       </c>
       <c r="I26">
         <v>0</v>
       </c>
       <c r="J26">
-        <v>0.002120294100004973</v>
+        <v>0</v>
       </c>
       <c r="K26" t="s">
         <v>49</v>
@@ -2358,19 +2358,19 @@
         <v>0</v>
       </c>
       <c r="R26">
-        <v>0</v>
+        <v>2.430912548402898</v>
       </c>
       <c r="S26">
-        <v>-0.02059537736770251</v>
+        <v>-0</v>
       </c>
       <c r="T26">
         <v>-0</v>
       </c>
       <c r="U26">
-        <v>0.02059537736770251</v>
+        <v>0</v>
       </c>
       <c r="V26">
-        <v>1.66</v>
+        <v>0</v>
       </c>
       <c r="W26">
         <v>0</v>
@@ -2384,7 +2384,7 @@
         <v>100.85</v>
       </c>
       <c r="C27">
-        <v>20.08286984699615</v>
+        <v>20</v>
       </c>
       <c r="D27">
         <v>0</v>
@@ -2396,7 +2396,7 @@
         <v>0</v>
       </c>
       <c r="G27">
-        <v>-0.26575992</v>
+        <v>0</v>
       </c>
       <c r="H27">
         <v>-0</v>
@@ -2441,7 +2441,7 @@
         <v>0</v>
       </c>
       <c r="V27">
-        <v>2.196</v>
+        <v>0</v>
       </c>
       <c r="W27">
         <v>0</v>

</xml_diff>